<commit_message>
Number of Vide for Train and Test for Par 4 and 5 done
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
+++ b/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE2D214-EEF6-4B2E-AABC-F8CF359CA3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -366,7 +367,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -431,7 +432,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -449,276 +450,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1052,23 +783,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +843,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1126,8 +857,12 @@
         <v>24</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="4">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4">
+        <v>24</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="J2" s="4">
         <v>6</v>
@@ -1136,11 +871,15 @@
         <v>6</v>
       </c>
       <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="M2" s="4">
+        <v>6</v>
+      </c>
+      <c r="N2" s="4">
+        <v>6</v>
+      </c>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1154,8 +893,12 @@
         <v>25</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="F3" s="4">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4">
+        <v>24</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="J3" s="4">
         <v>6</v>
@@ -1164,11 +907,15 @@
         <v>6</v>
       </c>
       <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="M3" s="4">
+        <v>6</v>
+      </c>
+      <c r="N3" s="4">
+        <v>6</v>
+      </c>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1182,8 +929,12 @@
         <v>24</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="4">
+        <v>36</v>
+      </c>
+      <c r="G4" s="4">
+        <v>24</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="J4" s="4">
         <v>6</v>
@@ -1192,11 +943,15 @@
         <v>6</v>
       </c>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="M4" s="4">
+        <v>12</v>
+      </c>
+      <c r="N4" s="4">
+        <v>6</v>
+      </c>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1210,8 +965,12 @@
         <v>24</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="F5" s="4">
+        <v>25</v>
+      </c>
+      <c r="G5" s="4">
+        <v>24</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="J5" s="4">
         <v>6</v>
@@ -1220,11 +979,15 @@
         <v>6</v>
       </c>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="M5" s="4">
+        <v>6</v>
+      </c>
+      <c r="N5" s="4">
+        <v>6</v>
+      </c>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1238,8 +1001,12 @@
         <v>37</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="4">
+        <v>23</v>
+      </c>
+      <c r="G6" s="4">
+        <v>24</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="J6" s="4">
         <v>7</v>
@@ -1248,11 +1015,15 @@
         <v>8</v>
       </c>
       <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="M6" s="4">
+        <v>8</v>
+      </c>
+      <c r="N6" s="4">
+        <v>6</v>
+      </c>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1266,8 +1037,12 @@
         <v>26</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="F7" s="4">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4">
+        <v>24</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="J7" s="4">
         <v>5</v>
@@ -1276,11 +1051,15 @@
         <v>6</v>
       </c>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="M7" s="4">
+        <v>6</v>
+      </c>
+      <c r="N7" s="4">
+        <v>6</v>
+      </c>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1294,8 +1073,12 @@
         <v>35</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="4">
+        <v>25</v>
+      </c>
+      <c r="G8" s="4">
+        <v>24</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="J8" s="4">
         <v>10</v>
@@ -1304,11 +1087,15 @@
         <v>10</v>
       </c>
       <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="M8" s="4">
+        <v>6</v>
+      </c>
+      <c r="N8" s="4">
+        <v>6</v>
+      </c>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1322,8 +1109,12 @@
         <v>24</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="F9" s="4">
+        <v>28</v>
+      </c>
+      <c r="G9" s="4">
+        <v>24</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="J9" s="4">
         <v>10</v>
@@ -1332,11 +1123,15 @@
         <v>6</v>
       </c>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="M9" s="4">
+        <v>6</v>
+      </c>
+      <c r="N9" s="4">
+        <v>6</v>
+      </c>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1350,8 +1145,12 @@
         <v>24</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="F10" s="4">
+        <v>24</v>
+      </c>
+      <c r="G10" s="4">
+        <v>24</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="J10" s="4">
         <v>6</v>
@@ -1360,11 +1159,15 @@
         <v>6</v>
       </c>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="M10" s="4">
+        <v>6</v>
+      </c>
+      <c r="N10" s="4">
+        <v>6</v>
+      </c>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1378,8 +1181,12 @@
         <v>24</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="F11" s="4">
+        <v>27</v>
+      </c>
+      <c r="G11" s="4">
+        <v>24</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="J11" s="4">
         <v>6</v>
@@ -1388,11 +1195,15 @@
         <v>6</v>
       </c>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="M11" s="4">
+        <v>6</v>
+      </c>
+      <c r="N11" s="4">
+        <v>6</v>
+      </c>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1406,8 +1217,12 @@
         <v>24</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="4">
+        <v>25</v>
+      </c>
+      <c r="G12" s="4">
+        <v>24</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="J12" s="4">
         <v>6</v>
@@ -1416,11 +1231,15 @@
         <v>6</v>
       </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="M12" s="4">
+        <v>6</v>
+      </c>
+      <c r="N12" s="4">
+        <v>6</v>
+      </c>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1434,8 +1253,12 @@
         <v>26</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="F13" s="4">
+        <v>25</v>
+      </c>
+      <c r="G13" s="4">
+        <v>24</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="J13" s="4">
         <v>6</v>
@@ -1444,11 +1267,15 @@
         <v>6</v>
       </c>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="M13" s="4">
+        <v>6</v>
+      </c>
+      <c r="N13" s="4">
+        <v>6</v>
+      </c>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1462,8 +1289,12 @@
         <v>16</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="F14" s="4">
+        <v>25</v>
+      </c>
+      <c r="G14" s="4">
+        <v>24</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="J14" s="4">
         <v>6</v>
@@ -1472,11 +1303,15 @@
         <v>6</v>
       </c>
       <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="M14" s="4">
+        <v>6</v>
+      </c>
+      <c r="N14" s="4">
+        <v>6</v>
+      </c>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -1490,8 +1325,12 @@
         <v>25</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="F15" s="4">
+        <v>24</v>
+      </c>
+      <c r="G15" s="4">
+        <v>24</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="J15" s="4">
         <v>6</v>
@@ -1500,11 +1339,15 @@
         <v>6</v>
       </c>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="M15" s="4">
+        <v>6</v>
+      </c>
+      <c r="N15" s="4">
+        <v>6</v>
+      </c>
       <c r="O15" s="4"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1518,8 +1361,12 @@
         <v>24</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="F16" s="4">
+        <v>25</v>
+      </c>
+      <c r="G16" s="4">
+        <v>24</v>
+      </c>
       <c r="H16" s="4"/>
       <c r="J16" s="4">
         <v>6</v>
@@ -1528,11 +1375,15 @@
         <v>6</v>
       </c>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="M16" s="4">
+        <v>6</v>
+      </c>
+      <c r="N16" s="4">
+        <v>6</v>
+      </c>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1546,8 +1397,12 @@
         <v>24</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="F17" s="4">
+        <v>25</v>
+      </c>
+      <c r="G17" s="4">
+        <v>24</v>
+      </c>
       <c r="H17" s="4"/>
       <c r="J17" s="4">
         <v>6</v>
@@ -1556,11 +1411,15 @@
         <v>6</v>
       </c>
       <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="M17" s="4">
+        <v>6</v>
+      </c>
+      <c r="N17" s="4">
+        <v>6</v>
+      </c>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1574,8 +1433,12 @@
         <v>24</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="F18" s="4">
+        <v>27</v>
+      </c>
+      <c r="G18" s="4">
+        <v>24</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="J18" s="4">
         <v>6</v>
@@ -1584,11 +1447,15 @@
         <v>6</v>
       </c>
       <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="M18" s="4">
+        <v>6</v>
+      </c>
+      <c r="N18" s="4">
+        <v>6</v>
+      </c>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1602,8 +1469,12 @@
         <v>24</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="F19" s="4">
+        <v>24</v>
+      </c>
+      <c r="G19" s="4">
+        <v>24</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="J19" s="4">
         <v>6</v>
@@ -1612,11 +1483,15 @@
         <v>6</v>
       </c>
       <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="M19" s="4">
+        <v>6</v>
+      </c>
+      <c r="N19" s="4">
+        <v>6</v>
+      </c>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -1630,8 +1505,12 @@
         <v>25</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="F20" s="4">
+        <v>25</v>
+      </c>
+      <c r="G20" s="4">
+        <v>24</v>
+      </c>
       <c r="H20" s="4"/>
       <c r="J20" s="4">
         <v>6</v>
@@ -1640,11 +1519,15 @@
         <v>6</v>
       </c>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
+      <c r="M20" s="4">
+        <v>6</v>
+      </c>
+      <c r="N20" s="4">
+        <v>6</v>
+      </c>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1658,8 +1541,12 @@
         <v>23</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="F21" s="4">
+        <v>25</v>
+      </c>
+      <c r="G21" s="4">
+        <v>24</v>
+      </c>
       <c r="H21" s="4"/>
       <c r="J21" s="4">
         <v>6</v>
@@ -1668,11 +1555,15 @@
         <v>6</v>
       </c>
       <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
+      <c r="M21" s="4">
+        <v>6</v>
+      </c>
+      <c r="N21" s="4">
+        <v>6</v>
+      </c>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1686,8 +1577,12 @@
         <v>24</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="F22" s="4">
+        <v>24</v>
+      </c>
+      <c r="G22" s="4">
+        <v>24</v>
+      </c>
       <c r="H22" s="4"/>
       <c r="J22" s="4">
         <v>6</v>
@@ -1696,11 +1591,15 @@
         <v>6</v>
       </c>
       <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+      <c r="M22" s="4">
+        <v>6</v>
+      </c>
+      <c r="N22" s="4">
+        <v>6</v>
+      </c>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1714,8 +1613,12 @@
         <v>25</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="F23" s="4">
+        <v>24</v>
+      </c>
+      <c r="G23" s="4">
+        <v>24</v>
+      </c>
       <c r="H23" s="4"/>
       <c r="J23" s="4">
         <v>6</v>
@@ -1724,11 +1627,15 @@
         <v>6</v>
       </c>
       <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
+      <c r="M23" s="4">
+        <v>6</v>
+      </c>
+      <c r="N23" s="4">
+        <v>6</v>
+      </c>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -1742,8 +1649,12 @@
         <v>25</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="F24" s="4">
+        <v>24</v>
+      </c>
+      <c r="G24" s="4">
+        <v>24</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="J24" s="4">
         <v>6</v>
@@ -1752,11 +1663,15 @@
         <v>6</v>
       </c>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
+      <c r="M24" s="4">
+        <v>6</v>
+      </c>
+      <c r="N24" s="4">
+        <v>6</v>
+      </c>
       <c r="O24" s="4"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -1770,8 +1685,12 @@
         <v>25</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="F25" s="4">
+        <v>24</v>
+      </c>
+      <c r="G25" s="4">
+        <v>24</v>
+      </c>
       <c r="H25" s="4"/>
       <c r="J25" s="4">
         <v>6</v>
@@ -1780,11 +1699,15 @@
         <v>6</v>
       </c>
       <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
+      <c r="M25" s="4">
+        <v>6</v>
+      </c>
+      <c r="N25" s="4">
+        <v>6</v>
+      </c>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -1798,8 +1721,12 @@
         <v>24</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="F26" s="4">
+        <v>25</v>
+      </c>
+      <c r="G26" s="4">
+        <v>24</v>
+      </c>
       <c r="H26" s="4"/>
       <c r="J26" s="4">
         <v>6</v>
@@ -1808,11 +1735,15 @@
         <v>6</v>
       </c>
       <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
+      <c r="M26" s="4">
+        <v>6</v>
+      </c>
+      <c r="N26" s="4">
+        <v>6</v>
+      </c>
       <c r="O26" s="4"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -1826,8 +1757,12 @@
         <v>24</v>
       </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="F27" s="4">
+        <v>25</v>
+      </c>
+      <c r="G27" s="4">
+        <v>24</v>
+      </c>
       <c r="H27" s="4"/>
       <c r="J27" s="4">
         <v>6</v>
@@ -1836,11 +1771,15 @@
         <v>6</v>
       </c>
       <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
+      <c r="M27" s="4">
+        <v>6</v>
+      </c>
+      <c r="N27" s="4">
+        <v>6</v>
+      </c>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
@@ -1854,8 +1793,12 @@
         <v>51</v>
       </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="F28" s="4">
+        <v>24</v>
+      </c>
+      <c r="G28" s="4">
+        <v>24</v>
+      </c>
       <c r="H28" s="4"/>
       <c r="J28" s="4">
         <v>6</v>
@@ -1864,11 +1807,15 @@
         <v>10</v>
       </c>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
+      <c r="M28" s="4">
+        <v>6</v>
+      </c>
+      <c r="N28" s="4">
+        <v>6</v>
+      </c>
       <c r="O28" s="4"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -1882,8 +1829,12 @@
         <v>45</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="F29" s="4">
+        <v>24</v>
+      </c>
+      <c r="G29" s="4">
+        <v>24</v>
+      </c>
       <c r="H29" s="4"/>
       <c r="J29" s="4">
         <v>6</v>
@@ -1892,11 +1843,15 @@
         <v>16</v>
       </c>
       <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
+      <c r="M29" s="4">
+        <v>6</v>
+      </c>
+      <c r="N29" s="4">
+        <v>6</v>
+      </c>
       <c r="O29" s="4"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -1910,8 +1865,12 @@
         <v>24</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="F30" s="4">
+        <v>24</v>
+      </c>
+      <c r="G30" s="4">
+        <v>24</v>
+      </c>
       <c r="H30" s="4"/>
       <c r="J30" s="4">
         <v>6</v>
@@ -1920,11 +1879,15 @@
         <v>6</v>
       </c>
       <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
+      <c r="M30" s="4">
+        <v>6</v>
+      </c>
+      <c r="N30" s="4">
+        <v>6</v>
+      </c>
       <c r="O30" s="4"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -1938,8 +1901,12 @@
         <v>25</v>
       </c>
       <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="F31" s="4">
+        <v>24</v>
+      </c>
+      <c r="G31" s="4">
+        <v>24</v>
+      </c>
       <c r="H31" s="4"/>
       <c r="J31" s="4">
         <v>6</v>
@@ -1948,11 +1915,15 @@
         <v>6</v>
       </c>
       <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
+      <c r="M31" s="4">
+        <v>6</v>
+      </c>
+      <c r="N31" s="4">
+        <v>6</v>
+      </c>
       <c r="O31" s="4"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -1966,8 +1937,12 @@
         <v>24</v>
       </c>
       <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="F32" s="4">
+        <v>25</v>
+      </c>
+      <c r="G32" s="4">
+        <v>24</v>
+      </c>
       <c r="H32" s="4"/>
       <c r="J32" s="4">
         <v>6</v>
@@ -1976,11 +1951,15 @@
         <v>6</v>
       </c>
       <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
+      <c r="M32" s="4">
+        <v>6</v>
+      </c>
+      <c r="N32" s="4">
+        <v>6</v>
+      </c>
       <c r="O32" s="4"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -1994,8 +1973,12 @@
         <v>24</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="F33" s="4">
+        <v>24</v>
+      </c>
+      <c r="G33" s="4">
+        <v>24</v>
+      </c>
       <c r="H33" s="4"/>
       <c r="J33" s="4">
         <v>6</v>
@@ -2004,11 +1987,15 @@
         <v>6</v>
       </c>
       <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
+      <c r="M33" s="4">
+        <v>6</v>
+      </c>
+      <c r="N33" s="4">
+        <v>6</v>
+      </c>
       <c r="O33" s="4"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -2022,8 +2009,12 @@
         <v>24</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="F34" s="4">
+        <v>24</v>
+      </c>
+      <c r="G34" s="4">
+        <v>24</v>
+      </c>
       <c r="H34" s="4"/>
       <c r="J34" s="4">
         <v>6</v>
@@ -2032,11 +2023,15 @@
         <v>6</v>
       </c>
       <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
+      <c r="M34" s="4">
+        <v>6</v>
+      </c>
+      <c r="N34" s="4">
+        <v>6</v>
+      </c>
       <c r="O34" s="4"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -2050,8 +2045,12 @@
         <v>25</v>
       </c>
       <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="F35" s="4">
+        <v>24</v>
+      </c>
+      <c r="G35" s="4">
+        <v>24</v>
+      </c>
       <c r="H35" s="4"/>
       <c r="J35" s="4">
         <v>6</v>
@@ -2060,11 +2059,15 @@
         <v>6</v>
       </c>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
+      <c r="M35" s="4">
+        <v>6</v>
+      </c>
+      <c r="N35" s="4">
+        <v>6</v>
+      </c>
       <c r="O35" s="4"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
@@ -2078,8 +2081,12 @@
         <v>24</v>
       </c>
       <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="F36" s="4">
+        <v>25</v>
+      </c>
+      <c r="G36" s="4">
+        <v>24</v>
+      </c>
       <c r="H36" s="4"/>
       <c r="J36" s="4">
         <v>6</v>
@@ -2088,11 +2095,15 @@
         <v>6</v>
       </c>
       <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
+      <c r="M36" s="4">
+        <v>6</v>
+      </c>
+      <c r="N36" s="4">
+        <v>6</v>
+      </c>
       <c r="O36" s="4"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -2106,8 +2117,12 @@
         <v>25</v>
       </c>
       <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="F37" s="4">
+        <v>24</v>
+      </c>
+      <c r="G37" s="4">
+        <v>24</v>
+      </c>
       <c r="H37" s="4"/>
       <c r="J37" s="4">
         <v>6</v>
@@ -2116,11 +2131,15 @@
         <v>6</v>
       </c>
       <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
+      <c r="M37" s="4">
+        <v>6</v>
+      </c>
+      <c r="N37" s="4">
+        <v>6</v>
+      </c>
       <c r="O37" s="4"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -2134,8 +2153,12 @@
         <v>24</v>
       </c>
       <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="F38" s="4">
+        <v>24</v>
+      </c>
+      <c r="G38" s="4">
+        <v>24</v>
+      </c>
       <c r="H38" s="4"/>
       <c r="J38" s="4">
         <v>6</v>
@@ -2144,11 +2167,15 @@
         <v>6</v>
       </c>
       <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
+      <c r="M38" s="4">
+        <v>6</v>
+      </c>
+      <c r="N38" s="4">
+        <v>6</v>
+      </c>
       <c r="O38" s="4"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -2162,8 +2189,12 @@
         <v>24</v>
       </c>
       <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="F39" s="4">
+        <v>24</v>
+      </c>
+      <c r="G39" s="4">
+        <v>24</v>
+      </c>
       <c r="H39" s="4"/>
       <c r="J39" s="4">
         <v>6</v>
@@ -2172,11 +2203,15 @@
         <v>6</v>
       </c>
       <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
+      <c r="M39" s="4">
+        <v>6</v>
+      </c>
+      <c r="N39" s="4">
+        <v>6</v>
+      </c>
       <c r="O39" s="4"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
@@ -2190,8 +2225,12 @@
         <v>24</v>
       </c>
       <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="F40" s="4">
+        <v>24</v>
+      </c>
+      <c r="G40" s="4">
+        <v>24</v>
+      </c>
       <c r="H40" s="4"/>
       <c r="J40" s="4">
         <v>6</v>
@@ -2200,11 +2239,15 @@
         <v>6</v>
       </c>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
+      <c r="M40" s="4">
+        <v>6</v>
+      </c>
+      <c r="N40" s="4">
+        <v>6</v>
+      </c>
       <c r="O40" s="4"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
@@ -2218,8 +2261,12 @@
         <v>25</v>
       </c>
       <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="F41" s="4">
+        <v>24</v>
+      </c>
+      <c r="G41" s="4">
+        <v>24</v>
+      </c>
       <c r="H41" s="4"/>
       <c r="J41" s="4">
         <v>6</v>
@@ -2228,11 +2275,15 @@
         <v>6</v>
       </c>
       <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
+      <c r="M41" s="4">
+        <v>6</v>
+      </c>
+      <c r="N41" s="4">
+        <v>6</v>
+      </c>
       <c r="O41" s="4"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -2246,8 +2297,12 @@
         <v>25</v>
       </c>
       <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="F42" s="4">
+        <v>24</v>
+      </c>
+      <c r="G42" s="4">
+        <v>24</v>
+      </c>
       <c r="H42" s="4"/>
       <c r="J42" s="4">
         <v>6</v>
@@ -2256,11 +2311,15 @@
         <v>6</v>
       </c>
       <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
+      <c r="M42" s="4">
+        <v>6</v>
+      </c>
+      <c r="N42" s="4">
+        <v>6</v>
+      </c>
       <c r="O42" s="4"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -2274,8 +2333,12 @@
         <v>24</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="F43" s="4">
+        <v>24</v>
+      </c>
+      <c r="G43" s="4">
+        <v>23</v>
+      </c>
       <c r="H43" s="4"/>
       <c r="J43" s="4">
         <v>6</v>
@@ -2284,11 +2347,15 @@
         <v>6</v>
       </c>
       <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
+      <c r="M43" s="4">
+        <v>6</v>
+      </c>
+      <c r="N43" s="4">
+        <v>6</v>
+      </c>
       <c r="O43" s="4"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -2302,8 +2369,12 @@
         <v>24</v>
       </c>
       <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="F44" s="4">
+        <v>25</v>
+      </c>
+      <c r="G44" s="4">
+        <v>24</v>
+      </c>
       <c r="H44" s="4"/>
       <c r="J44" s="4">
         <v>6</v>
@@ -2312,11 +2383,15 @@
         <v>6</v>
       </c>
       <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
+      <c r="M44" s="4">
+        <v>6</v>
+      </c>
+      <c r="N44" s="4">
+        <v>6</v>
+      </c>
       <c r="O44" s="4"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -2330,8 +2405,12 @@
         <v>24</v>
       </c>
       <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="F45" s="4">
+        <v>24</v>
+      </c>
+      <c r="G45" s="4">
+        <v>24</v>
+      </c>
       <c r="H45" s="4"/>
       <c r="J45" s="4">
         <v>5</v>
@@ -2340,11 +2419,15 @@
         <v>6</v>
       </c>
       <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
+      <c r="M45" s="4">
+        <v>6</v>
+      </c>
+      <c r="N45" s="4">
+        <v>6</v>
+      </c>
       <c r="O45" s="4"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>90</v>
       </c>
@@ -2358,8 +2441,12 @@
         <v>24</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+      <c r="F46" s="4">
+        <v>24</v>
+      </c>
+      <c r="G46" s="4">
+        <v>24</v>
+      </c>
       <c r="H46" s="4"/>
       <c r="J46" s="4">
         <v>6</v>
@@ -2368,11 +2455,15 @@
         <v>6</v>
       </c>
       <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
+      <c r="M46" s="4">
+        <v>6</v>
+      </c>
+      <c r="N46" s="4">
+        <v>6</v>
+      </c>
       <c r="O46" s="4"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
@@ -2386,8 +2477,12 @@
         <v>24</v>
       </c>
       <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
+      <c r="F47" s="4">
+        <v>24</v>
+      </c>
+      <c r="G47" s="4">
+        <v>24</v>
+      </c>
       <c r="H47" s="4"/>
       <c r="J47" s="4">
         <v>6</v>
@@ -2396,11 +2491,15 @@
         <v>6</v>
       </c>
       <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
+      <c r="M47" s="4">
+        <v>6</v>
+      </c>
+      <c r="N47" s="4">
+        <v>6</v>
+      </c>
       <c r="O47" s="4"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -2414,8 +2513,12 @@
         <v>24</v>
       </c>
       <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
+      <c r="F48" s="4">
+        <v>24</v>
+      </c>
+      <c r="G48" s="4">
+        <v>24</v>
+      </c>
       <c r="H48" s="4"/>
       <c r="J48" s="4">
         <v>6</v>
@@ -2424,11 +2527,15 @@
         <v>6</v>
       </c>
       <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
+      <c r="M48" s="4">
+        <v>6</v>
+      </c>
+      <c r="N48" s="4">
+        <v>6</v>
+      </c>
       <c r="O48" s="4"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -2442,8 +2549,12 @@
         <v>24</v>
       </c>
       <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
+      <c r="F49" s="4">
+        <v>24</v>
+      </c>
+      <c r="G49" s="4">
+        <v>24</v>
+      </c>
       <c r="H49" s="4"/>
       <c r="J49" s="4">
         <v>6</v>
@@ -2452,11 +2563,15 @@
         <v>6</v>
       </c>
       <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
+      <c r="M49" s="4">
+        <v>6</v>
+      </c>
+      <c r="N49" s="4">
+        <v>6</v>
+      </c>
       <c r="O49" s="4"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -2470,8 +2585,12 @@
         <v>24</v>
       </c>
       <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
+      <c r="F50" s="4">
+        <v>24</v>
+      </c>
+      <c r="G50" s="4">
+        <v>24</v>
+      </c>
       <c r="H50" s="4"/>
       <c r="J50" s="4">
         <v>6</v>
@@ -2480,11 +2599,15 @@
         <v>6</v>
       </c>
       <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
+      <c r="M50" s="4">
+        <v>6</v>
+      </c>
+      <c r="N50" s="4">
+        <v>6</v>
+      </c>
       <c r="O50" s="4"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -2498,8 +2621,12 @@
         <v>24</v>
       </c>
       <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
+      <c r="F51" s="4">
+        <v>24</v>
+      </c>
+      <c r="G51" s="4">
+        <v>24</v>
+      </c>
       <c r="H51" s="4"/>
       <c r="J51" s="4">
         <v>6</v>
@@ -2508,34 +2635,38 @@
         <v>6</v>
       </c>
       <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
+      <c r="M51" s="4">
+        <v>6</v>
+      </c>
+      <c r="N51" s="4">
+        <v>6</v>
+      </c>
       <c r="O51" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:H51">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="between">
       <formula>22</formula>
       <formula>26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
       <formula>27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="lessThan">
       <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:O51">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added P6 training and testing
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
+++ b/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0603EE-90AD-7F47-8876-89EFCEBAAC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="860" yWindow="500" windowWidth="26020" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>SentenceID</t>
   </si>
@@ -361,12 +362,18 @@
   </si>
   <si>
     <t>P6 # Testing</t>
+  </si>
+  <si>
+    <t>* P6 blooper</t>
+  </si>
+  <si>
+    <t>*P6 has 1 dif signer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -431,7 +438,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -444,11 +461,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFAACAC"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -474,301 +501,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1052,23 +789,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="15" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +850,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1126,9 +864,15 @@
         <v>24</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="F2" s="4">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4">
+        <v>24</v>
+      </c>
+      <c r="H2" s="4">
+        <v>25</v>
+      </c>
       <c r="J2" s="4">
         <v>6</v>
       </c>
@@ -1136,11 +880,17 @@
         <v>6</v>
       </c>
       <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M2" s="4">
+        <v>6</v>
+      </c>
+      <c r="N2" s="4">
+        <v>6</v>
+      </c>
+      <c r="O2" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1154,9 +904,15 @@
         <v>25</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="F3" s="4">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4">
+        <v>24</v>
+      </c>
+      <c r="H3" s="4">
+        <v>26</v>
+      </c>
       <c r="J3" s="4">
         <v>6</v>
       </c>
@@ -1164,11 +920,17 @@
         <v>6</v>
       </c>
       <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M3" s="4">
+        <v>6</v>
+      </c>
+      <c r="N3" s="4">
+        <v>6</v>
+      </c>
+      <c r="O3" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1182,9 +944,15 @@
         <v>24</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="F4" s="4">
+        <v>36</v>
+      </c>
+      <c r="G4" s="4">
+        <v>24</v>
+      </c>
+      <c r="H4" s="4">
+        <v>25</v>
+      </c>
       <c r="J4" s="4">
         <v>6</v>
       </c>
@@ -1192,11 +960,20 @@
         <v>6</v>
       </c>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M4" s="4">
+        <v>12</v>
+      </c>
+      <c r="N4" s="4">
+        <v>6</v>
+      </c>
+      <c r="O4" s="4">
+        <v>6</v>
+      </c>
+      <c r="P4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1210,9 +987,15 @@
         <v>24</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="F5" s="4">
+        <v>25</v>
+      </c>
+      <c r="G5" s="4">
+        <v>24</v>
+      </c>
+      <c r="H5" s="4">
+        <v>24</v>
+      </c>
       <c r="J5" s="4">
         <v>6</v>
       </c>
@@ -1220,11 +1003,17 @@
         <v>6</v>
       </c>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M5" s="4">
+        <v>6</v>
+      </c>
+      <c r="N5" s="4">
+        <v>6</v>
+      </c>
+      <c r="O5" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1238,9 +1027,15 @@
         <v>37</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="F6" s="4">
+        <v>23</v>
+      </c>
+      <c r="G6" s="4">
+        <v>24</v>
+      </c>
+      <c r="H6" s="4">
+        <v>23</v>
+      </c>
       <c r="J6" s="4">
         <v>7</v>
       </c>
@@ -1248,11 +1043,17 @@
         <v>8</v>
       </c>
       <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M6" s="4">
+        <v>8</v>
+      </c>
+      <c r="N6" s="4">
+        <v>6</v>
+      </c>
+      <c r="O6" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1266,9 +1067,15 @@
         <v>26</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="F7" s="4">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4">
+        <v>24</v>
+      </c>
+      <c r="H7" s="4">
+        <v>24</v>
+      </c>
       <c r="J7" s="4">
         <v>5</v>
       </c>
@@ -1276,11 +1083,17 @@
         <v>6</v>
       </c>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M7" s="4">
+        <v>6</v>
+      </c>
+      <c r="N7" s="4">
+        <v>6</v>
+      </c>
+      <c r="O7" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1294,9 +1107,15 @@
         <v>35</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="F8" s="4">
+        <v>25</v>
+      </c>
+      <c r="G8" s="4">
+        <v>24</v>
+      </c>
+      <c r="H8" s="4">
+        <v>24</v>
+      </c>
       <c r="J8" s="4">
         <v>10</v>
       </c>
@@ -1304,11 +1123,17 @@
         <v>10</v>
       </c>
       <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M8" s="4">
+        <v>6</v>
+      </c>
+      <c r="N8" s="4">
+        <v>6</v>
+      </c>
+      <c r="O8" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1322,9 +1147,15 @@
         <v>24</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="F9" s="4">
+        <v>28</v>
+      </c>
+      <c r="G9" s="4">
+        <v>24</v>
+      </c>
+      <c r="H9" s="4">
+        <v>24</v>
+      </c>
       <c r="J9" s="4">
         <v>10</v>
       </c>
@@ -1332,11 +1163,17 @@
         <v>6</v>
       </c>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M9" s="4">
+        <v>6</v>
+      </c>
+      <c r="N9" s="4">
+        <v>6</v>
+      </c>
+      <c r="O9" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1350,9 +1187,15 @@
         <v>24</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="F10" s="4">
+        <v>24</v>
+      </c>
+      <c r="G10" s="4">
+        <v>24</v>
+      </c>
+      <c r="H10" s="4">
+        <v>24</v>
+      </c>
       <c r="J10" s="4">
         <v>6</v>
       </c>
@@ -1360,11 +1203,17 @@
         <v>6</v>
       </c>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M10" s="4">
+        <v>6</v>
+      </c>
+      <c r="N10" s="4">
+        <v>6</v>
+      </c>
+      <c r="O10" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1378,9 +1227,15 @@
         <v>24</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="F11" s="4">
+        <v>27</v>
+      </c>
+      <c r="G11" s="4">
+        <v>24</v>
+      </c>
+      <c r="H11" s="4">
+        <v>24</v>
+      </c>
       <c r="J11" s="4">
         <v>6</v>
       </c>
@@ -1388,11 +1243,17 @@
         <v>6</v>
       </c>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M11" s="4">
+        <v>6</v>
+      </c>
+      <c r="N11" s="4">
+        <v>6</v>
+      </c>
+      <c r="O11" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1406,9 +1267,15 @@
         <v>24</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="F12" s="4">
+        <v>25</v>
+      </c>
+      <c r="G12" s="4">
+        <v>24</v>
+      </c>
+      <c r="H12" s="4">
+        <v>24</v>
+      </c>
       <c r="J12" s="4">
         <v>6</v>
       </c>
@@ -1416,11 +1283,17 @@
         <v>6</v>
       </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M12" s="4">
+        <v>6</v>
+      </c>
+      <c r="N12" s="4">
+        <v>6</v>
+      </c>
+      <c r="O12" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1434,9 +1307,15 @@
         <v>26</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="F13" s="4">
+        <v>25</v>
+      </c>
+      <c r="G13" s="4">
+        <v>24</v>
+      </c>
+      <c r="H13" s="4">
+        <v>25</v>
+      </c>
       <c r="J13" s="4">
         <v>6</v>
       </c>
@@ -1444,11 +1323,17 @@
         <v>6</v>
       </c>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M13" s="4">
+        <v>6</v>
+      </c>
+      <c r="N13" s="4">
+        <v>6</v>
+      </c>
+      <c r="O13" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1462,9 +1347,15 @@
         <v>16</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="F14" s="4">
+        <v>25</v>
+      </c>
+      <c r="G14" s="4">
+        <v>24</v>
+      </c>
+      <c r="H14" s="4">
+        <v>24</v>
+      </c>
       <c r="J14" s="4">
         <v>6</v>
       </c>
@@ -1472,11 +1363,17 @@
         <v>6</v>
       </c>
       <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M14" s="4">
+        <v>6</v>
+      </c>
+      <c r="N14" s="4">
+        <v>6</v>
+      </c>
+      <c r="O14" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -1490,9 +1387,15 @@
         <v>25</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="F15" s="4">
+        <v>24</v>
+      </c>
+      <c r="G15" s="4">
+        <v>24</v>
+      </c>
+      <c r="H15" s="4">
+        <v>25</v>
+      </c>
       <c r="J15" s="4">
         <v>6</v>
       </c>
@@ -1500,11 +1403,17 @@
         <v>6</v>
       </c>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M15" s="4">
+        <v>6</v>
+      </c>
+      <c r="N15" s="4">
+        <v>6</v>
+      </c>
+      <c r="O15" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1518,9 +1427,15 @@
         <v>24</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="F16" s="4">
+        <v>25</v>
+      </c>
+      <c r="G16" s="4">
+        <v>24</v>
+      </c>
+      <c r="H16" s="4">
+        <v>24</v>
+      </c>
       <c r="J16" s="4">
         <v>6</v>
       </c>
@@ -1528,11 +1443,17 @@
         <v>6</v>
       </c>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M16" s="4">
+        <v>6</v>
+      </c>
+      <c r="N16" s="4">
+        <v>6</v>
+      </c>
+      <c r="O16" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1546,9 +1467,15 @@
         <v>24</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="F17" s="4">
+        <v>25</v>
+      </c>
+      <c r="G17" s="4">
+        <v>24</v>
+      </c>
+      <c r="H17" s="4">
+        <v>24</v>
+      </c>
       <c r="J17" s="4">
         <v>6</v>
       </c>
@@ -1556,11 +1483,17 @@
         <v>6</v>
       </c>
       <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M17" s="4">
+        <v>6</v>
+      </c>
+      <c r="N17" s="4">
+        <v>6</v>
+      </c>
+      <c r="O17" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1574,9 +1507,15 @@
         <v>24</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="F18" s="4">
+        <v>27</v>
+      </c>
+      <c r="G18" s="4">
+        <v>24</v>
+      </c>
+      <c r="H18" s="4">
+        <v>24</v>
+      </c>
       <c r="J18" s="4">
         <v>6</v>
       </c>
@@ -1584,11 +1523,17 @@
         <v>6</v>
       </c>
       <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M18" s="4">
+        <v>6</v>
+      </c>
+      <c r="N18" s="4">
+        <v>6</v>
+      </c>
+      <c r="O18" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1602,9 +1547,15 @@
         <v>24</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="F19" s="4">
+        <v>24</v>
+      </c>
+      <c r="G19" s="4">
+        <v>24</v>
+      </c>
+      <c r="H19" s="4">
+        <v>24</v>
+      </c>
       <c r="J19" s="4">
         <v>6</v>
       </c>
@@ -1612,11 +1563,17 @@
         <v>6</v>
       </c>
       <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M19" s="4">
+        <v>6</v>
+      </c>
+      <c r="N19" s="4">
+        <v>6</v>
+      </c>
+      <c r="O19" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -1630,9 +1587,15 @@
         <v>25</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="F20" s="4">
+        <v>25</v>
+      </c>
+      <c r="G20" s="4">
+        <v>24</v>
+      </c>
+      <c r="H20" s="4">
+        <v>24</v>
+      </c>
       <c r="J20" s="4">
         <v>6</v>
       </c>
@@ -1640,11 +1603,17 @@
         <v>6</v>
       </c>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M20" s="4">
+        <v>6</v>
+      </c>
+      <c r="N20" s="4">
+        <v>6</v>
+      </c>
+      <c r="O20" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1658,9 +1627,15 @@
         <v>23</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="F21" s="4">
+        <v>25</v>
+      </c>
+      <c r="G21" s="4">
+        <v>24</v>
+      </c>
+      <c r="H21" s="4">
+        <v>24</v>
+      </c>
       <c r="J21" s="4">
         <v>6</v>
       </c>
@@ -1668,11 +1643,17 @@
         <v>6</v>
       </c>
       <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M21" s="4">
+        <v>6</v>
+      </c>
+      <c r="N21" s="4">
+        <v>6</v>
+      </c>
+      <c r="O21" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1686,9 +1667,15 @@
         <v>24</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="F22" s="4">
+        <v>24</v>
+      </c>
+      <c r="G22" s="4">
+        <v>24</v>
+      </c>
+      <c r="H22" s="4">
+        <v>24</v>
+      </c>
       <c r="J22" s="4">
         <v>6</v>
       </c>
@@ -1696,11 +1683,17 @@
         <v>6</v>
       </c>
       <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M22" s="4">
+        <v>6</v>
+      </c>
+      <c r="N22" s="4">
+        <v>6</v>
+      </c>
+      <c r="O22" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1714,9 +1707,15 @@
         <v>25</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="F23" s="4">
+        <v>24</v>
+      </c>
+      <c r="G23" s="4">
+        <v>24</v>
+      </c>
+      <c r="H23" s="4">
+        <v>25</v>
+      </c>
       <c r="J23" s="4">
         <v>6</v>
       </c>
@@ -1724,11 +1723,17 @@
         <v>6</v>
       </c>
       <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M23" s="4">
+        <v>6</v>
+      </c>
+      <c r="N23" s="4">
+        <v>6</v>
+      </c>
+      <c r="O23" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -1742,9 +1747,15 @@
         <v>25</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="F24" s="4">
+        <v>24</v>
+      </c>
+      <c r="G24" s="4">
+        <v>24</v>
+      </c>
+      <c r="H24" s="4">
+        <v>26</v>
+      </c>
       <c r="J24" s="4">
         <v>6</v>
       </c>
@@ -1752,11 +1763,17 @@
         <v>6</v>
       </c>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M24" s="4">
+        <v>6</v>
+      </c>
+      <c r="N24" s="4">
+        <v>6</v>
+      </c>
+      <c r="O24" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -1770,9 +1787,15 @@
         <v>25</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="F25" s="4">
+        <v>24</v>
+      </c>
+      <c r="G25" s="4">
+        <v>24</v>
+      </c>
+      <c r="H25" s="4">
+        <v>24</v>
+      </c>
       <c r="J25" s="4">
         <v>6</v>
       </c>
@@ -1780,11 +1803,17 @@
         <v>6</v>
       </c>
       <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M25" s="4">
+        <v>6</v>
+      </c>
+      <c r="N25" s="4">
+        <v>6</v>
+      </c>
+      <c r="O25" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -1798,9 +1827,15 @@
         <v>24</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="F26" s="4">
+        <v>25</v>
+      </c>
+      <c r="G26" s="4">
+        <v>24</v>
+      </c>
+      <c r="H26" s="4">
+        <v>26</v>
+      </c>
       <c r="J26" s="4">
         <v>6</v>
       </c>
@@ -1808,11 +1843,17 @@
         <v>6</v>
       </c>
       <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M26" s="4">
+        <v>6</v>
+      </c>
+      <c r="N26" s="4">
+        <v>6</v>
+      </c>
+      <c r="O26" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -1826,9 +1867,15 @@
         <v>24</v>
       </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="F27" s="4">
+        <v>25</v>
+      </c>
+      <c r="G27" s="4">
+        <v>24</v>
+      </c>
+      <c r="H27" s="4">
+        <v>25</v>
+      </c>
       <c r="J27" s="4">
         <v>6</v>
       </c>
@@ -1836,11 +1883,17 @@
         <v>6</v>
       </c>
       <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M27" s="4">
+        <v>6</v>
+      </c>
+      <c r="N27" s="4">
+        <v>6</v>
+      </c>
+      <c r="O27" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
@@ -1854,9 +1907,15 @@
         <v>51</v>
       </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="F28" s="4">
+        <v>24</v>
+      </c>
+      <c r="G28" s="4">
+        <v>24</v>
+      </c>
+      <c r="H28" s="4">
+        <v>24</v>
+      </c>
       <c r="J28" s="4">
         <v>6</v>
       </c>
@@ -1864,11 +1923,17 @@
         <v>10</v>
       </c>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M28" s="4">
+        <v>6</v>
+      </c>
+      <c r="N28" s="4">
+        <v>6</v>
+      </c>
+      <c r="O28" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -1882,9 +1947,15 @@
         <v>45</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="F29" s="4">
+        <v>24</v>
+      </c>
+      <c r="G29" s="4">
+        <v>24</v>
+      </c>
+      <c r="H29" s="4">
+        <v>24</v>
+      </c>
       <c r="J29" s="4">
         <v>6</v>
       </c>
@@ -1892,11 +1963,17 @@
         <v>16</v>
       </c>
       <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M29" s="4">
+        <v>6</v>
+      </c>
+      <c r="N29" s="4">
+        <v>6</v>
+      </c>
+      <c r="O29" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -1910,9 +1987,15 @@
         <v>24</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="F30" s="4">
+        <v>24</v>
+      </c>
+      <c r="G30" s="4">
+        <v>24</v>
+      </c>
+      <c r="H30" s="4">
+        <v>24</v>
+      </c>
       <c r="J30" s="4">
         <v>6</v>
       </c>
@@ -1920,11 +2003,17 @@
         <v>6</v>
       </c>
       <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M30" s="4">
+        <v>6</v>
+      </c>
+      <c r="N30" s="4">
+        <v>6</v>
+      </c>
+      <c r="O30" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -1938,9 +2027,18 @@
         <v>25</v>
       </c>
       <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
+      <c r="F31" s="4">
+        <v>24</v>
+      </c>
+      <c r="G31" s="4">
+        <v>24</v>
+      </c>
+      <c r="H31" s="4">
+        <v>24</v>
+      </c>
+      <c r="I31" t="s">
+        <v>114</v>
+      </c>
       <c r="J31" s="4">
         <v>6</v>
       </c>
@@ -1948,11 +2046,17 @@
         <v>6</v>
       </c>
       <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M31" s="4">
+        <v>6</v>
+      </c>
+      <c r="N31" s="4">
+        <v>6</v>
+      </c>
+      <c r="O31" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -1966,9 +2070,15 @@
         <v>24</v>
       </c>
       <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+      <c r="F32" s="4">
+        <v>25</v>
+      </c>
+      <c r="G32" s="4">
+        <v>24</v>
+      </c>
+      <c r="H32" s="4">
+        <v>24</v>
+      </c>
       <c r="J32" s="4">
         <v>6</v>
       </c>
@@ -1976,11 +2086,17 @@
         <v>6</v>
       </c>
       <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M32" s="4">
+        <v>6</v>
+      </c>
+      <c r="N32" s="4">
+        <v>6</v>
+      </c>
+      <c r="O32" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -1994,9 +2110,15 @@
         <v>24</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+      <c r="F33" s="4">
+        <v>24</v>
+      </c>
+      <c r="G33" s="4">
+        <v>24</v>
+      </c>
+      <c r="H33" s="4">
+        <v>24</v>
+      </c>
       <c r="J33" s="4">
         <v>6</v>
       </c>
@@ -2004,11 +2126,17 @@
         <v>6</v>
       </c>
       <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M33" s="4">
+        <v>6</v>
+      </c>
+      <c r="N33" s="4">
+        <v>6</v>
+      </c>
+      <c r="O33" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -2022,9 +2150,15 @@
         <v>24</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="F34" s="4">
+        <v>24</v>
+      </c>
+      <c r="G34" s="4">
+        <v>24</v>
+      </c>
+      <c r="H34" s="4">
+        <v>25</v>
+      </c>
       <c r="J34" s="4">
         <v>6</v>
       </c>
@@ -2032,11 +2166,17 @@
         <v>6</v>
       </c>
       <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M34" s="4">
+        <v>6</v>
+      </c>
+      <c r="N34" s="4">
+        <v>6</v>
+      </c>
+      <c r="O34" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -2050,9 +2190,15 @@
         <v>25</v>
       </c>
       <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+      <c r="F35" s="4">
+        <v>24</v>
+      </c>
+      <c r="G35" s="4">
+        <v>24</v>
+      </c>
+      <c r="H35" s="4">
+        <v>24</v>
+      </c>
       <c r="J35" s="4">
         <v>6</v>
       </c>
@@ -2060,11 +2206,17 @@
         <v>6</v>
       </c>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M35" s="4">
+        <v>6</v>
+      </c>
+      <c r="N35" s="4">
+        <v>6</v>
+      </c>
+      <c r="O35" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
@@ -2078,9 +2230,15 @@
         <v>24</v>
       </c>
       <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
+      <c r="F36" s="4">
+        <v>25</v>
+      </c>
+      <c r="G36" s="4">
+        <v>24</v>
+      </c>
+      <c r="H36" s="4">
+        <v>24</v>
+      </c>
       <c r="J36" s="4">
         <v>6</v>
       </c>
@@ -2088,11 +2246,17 @@
         <v>6</v>
       </c>
       <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M36" s="4">
+        <v>6</v>
+      </c>
+      <c r="N36" s="4">
+        <v>6</v>
+      </c>
+      <c r="O36" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -2106,9 +2270,15 @@
         <v>25</v>
       </c>
       <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
+      <c r="F37" s="4">
+        <v>24</v>
+      </c>
+      <c r="G37" s="4">
+        <v>24</v>
+      </c>
+      <c r="H37" s="4">
+        <v>24</v>
+      </c>
       <c r="J37" s="4">
         <v>6</v>
       </c>
@@ -2116,11 +2286,17 @@
         <v>6</v>
       </c>
       <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M37" s="4">
+        <v>6</v>
+      </c>
+      <c r="N37" s="4">
+        <v>6</v>
+      </c>
+      <c r="O37" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -2134,9 +2310,15 @@
         <v>24</v>
       </c>
       <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
+      <c r="F38" s="4">
+        <v>24</v>
+      </c>
+      <c r="G38" s="4">
+        <v>24</v>
+      </c>
+      <c r="H38" s="4">
+        <v>24</v>
+      </c>
       <c r="J38" s="4">
         <v>6</v>
       </c>
@@ -2144,11 +2326,17 @@
         <v>6</v>
       </c>
       <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M38" s="4">
+        <v>6</v>
+      </c>
+      <c r="N38" s="4">
+        <v>6</v>
+      </c>
+      <c r="O38" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -2162,9 +2350,15 @@
         <v>24</v>
       </c>
       <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
+      <c r="F39" s="4">
+        <v>24</v>
+      </c>
+      <c r="G39" s="4">
+        <v>24</v>
+      </c>
+      <c r="H39" s="4">
+        <v>24</v>
+      </c>
       <c r="J39" s="4">
         <v>6</v>
       </c>
@@ -2172,11 +2366,17 @@
         <v>6</v>
       </c>
       <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M39" s="4">
+        <v>6</v>
+      </c>
+      <c r="N39" s="4">
+        <v>6</v>
+      </c>
+      <c r="O39" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
@@ -2190,9 +2390,15 @@
         <v>24</v>
       </c>
       <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
+      <c r="F40" s="4">
+        <v>24</v>
+      </c>
+      <c r="G40" s="4">
+        <v>24</v>
+      </c>
+      <c r="H40" s="4">
+        <v>24</v>
+      </c>
       <c r="J40" s="4">
         <v>6</v>
       </c>
@@ -2200,11 +2406,17 @@
         <v>6</v>
       </c>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M40" s="4">
+        <v>6</v>
+      </c>
+      <c r="N40" s="4">
+        <v>6</v>
+      </c>
+      <c r="O40" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
@@ -2218,9 +2430,15 @@
         <v>25</v>
       </c>
       <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
+      <c r="F41" s="4">
+        <v>24</v>
+      </c>
+      <c r="G41" s="4">
+        <v>24</v>
+      </c>
+      <c r="H41" s="4">
+        <v>24</v>
+      </c>
       <c r="J41" s="4">
         <v>6</v>
       </c>
@@ -2228,11 +2446,17 @@
         <v>6</v>
       </c>
       <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M41" s="4">
+        <v>6</v>
+      </c>
+      <c r="N41" s="4">
+        <v>6</v>
+      </c>
+      <c r="O41" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -2246,9 +2470,15 @@
         <v>25</v>
       </c>
       <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
+      <c r="F42" s="4">
+        <v>24</v>
+      </c>
+      <c r="G42" s="4">
+        <v>24</v>
+      </c>
+      <c r="H42" s="4">
+        <v>24</v>
+      </c>
       <c r="J42" s="4">
         <v>6</v>
       </c>
@@ -2256,11 +2486,17 @@
         <v>6</v>
       </c>
       <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M42" s="4">
+        <v>6</v>
+      </c>
+      <c r="N42" s="4">
+        <v>6</v>
+      </c>
+      <c r="O42" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -2274,9 +2510,15 @@
         <v>24</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
+      <c r="F43" s="4">
+        <v>24</v>
+      </c>
+      <c r="G43" s="4">
+        <v>23</v>
+      </c>
+      <c r="H43" s="4">
+        <v>24</v>
+      </c>
       <c r="J43" s="4">
         <v>6</v>
       </c>
@@ -2284,11 +2526,17 @@
         <v>6</v>
       </c>
       <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M43" s="4">
+        <v>6</v>
+      </c>
+      <c r="N43" s="4">
+        <v>6</v>
+      </c>
+      <c r="O43" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -2302,9 +2550,15 @@
         <v>24</v>
       </c>
       <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
+      <c r="F44" s="4">
+        <v>25</v>
+      </c>
+      <c r="G44" s="4">
+        <v>24</v>
+      </c>
+      <c r="H44" s="4">
+        <v>24</v>
+      </c>
       <c r="J44" s="4">
         <v>6</v>
       </c>
@@ -2312,11 +2566,17 @@
         <v>6</v>
       </c>
       <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M44" s="4">
+        <v>6</v>
+      </c>
+      <c r="N44" s="4">
+        <v>6</v>
+      </c>
+      <c r="O44" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -2330,9 +2590,15 @@
         <v>24</v>
       </c>
       <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
+      <c r="F45" s="4">
+        <v>24</v>
+      </c>
+      <c r="G45" s="4">
+        <v>24</v>
+      </c>
+      <c r="H45" s="4">
+        <v>24</v>
+      </c>
       <c r="J45" s="4">
         <v>5</v>
       </c>
@@ -2340,11 +2606,17 @@
         <v>6</v>
       </c>
       <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M45" s="4">
+        <v>6</v>
+      </c>
+      <c r="N45" s="4">
+        <v>6</v>
+      </c>
+      <c r="O45" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>90</v>
       </c>
@@ -2358,9 +2630,15 @@
         <v>24</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
+      <c r="F46" s="4">
+        <v>24</v>
+      </c>
+      <c r="G46" s="4">
+        <v>24</v>
+      </c>
+      <c r="H46" s="4">
+        <v>24</v>
+      </c>
       <c r="J46" s="4">
         <v>6</v>
       </c>
@@ -2368,11 +2646,17 @@
         <v>6</v>
       </c>
       <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M46" s="4">
+        <v>6</v>
+      </c>
+      <c r="N46" s="4">
+        <v>6</v>
+      </c>
+      <c r="O46" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
@@ -2386,9 +2670,15 @@
         <v>24</v>
       </c>
       <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
+      <c r="F47" s="4">
+        <v>24</v>
+      </c>
+      <c r="G47" s="4">
+        <v>24</v>
+      </c>
+      <c r="H47" s="4">
+        <v>24</v>
+      </c>
       <c r="J47" s="4">
         <v>6</v>
       </c>
@@ -2396,11 +2686,17 @@
         <v>6</v>
       </c>
       <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M47" s="4">
+        <v>6</v>
+      </c>
+      <c r="N47" s="4">
+        <v>6</v>
+      </c>
+      <c r="O47" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -2414,9 +2710,15 @@
         <v>24</v>
       </c>
       <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
+      <c r="F48" s="4">
+        <v>24</v>
+      </c>
+      <c r="G48" s="4">
+        <v>24</v>
+      </c>
+      <c r="H48" s="4">
+        <v>24</v>
+      </c>
       <c r="J48" s="4">
         <v>6</v>
       </c>
@@ -2424,11 +2726,17 @@
         <v>6</v>
       </c>
       <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M48" s="4">
+        <v>6</v>
+      </c>
+      <c r="N48" s="4">
+        <v>6</v>
+      </c>
+      <c r="O48" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -2442,9 +2750,15 @@
         <v>24</v>
       </c>
       <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
+      <c r="F49" s="4">
+        <v>24</v>
+      </c>
+      <c r="G49" s="4">
+        <v>24</v>
+      </c>
+      <c r="H49" s="4">
+        <v>24</v>
+      </c>
       <c r="J49" s="4">
         <v>6</v>
       </c>
@@ -2452,11 +2766,17 @@
         <v>6</v>
       </c>
       <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M49" s="4">
+        <v>6</v>
+      </c>
+      <c r="N49" s="4">
+        <v>6</v>
+      </c>
+      <c r="O49" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -2470,9 +2790,15 @@
         <v>24</v>
       </c>
       <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
+      <c r="F50" s="4">
+        <v>24</v>
+      </c>
+      <c r="G50" s="4">
+        <v>24</v>
+      </c>
+      <c r="H50" s="4">
+        <v>24</v>
+      </c>
       <c r="J50" s="4">
         <v>6</v>
       </c>
@@ -2480,11 +2806,17 @@
         <v>6</v>
       </c>
       <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M50" s="4">
+        <v>6</v>
+      </c>
+      <c r="N50" s="4">
+        <v>6</v>
+      </c>
+      <c r="O50" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -2498,9 +2830,15 @@
         <v>24</v>
       </c>
       <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
+      <c r="F51" s="4">
+        <v>24</v>
+      </c>
+      <c r="G51" s="4">
+        <v>24</v>
+      </c>
+      <c r="H51" s="4">
+        <v>24</v>
+      </c>
       <c r="J51" s="4">
         <v>6</v>
       </c>
@@ -2508,34 +2846,40 @@
         <v>6</v>
       </c>
       <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
+      <c r="M51" s="4">
+        <v>6</v>
+      </c>
+      <c r="N51" s="4">
+        <v>6</v>
+      </c>
+      <c r="O51" s="4">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:H51">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="greaterThan">
+      <formula>27</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
       <formula>22</formula>
       <formula>26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="lessThan">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>27</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
-      <formula>27</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
-      <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:O51">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
P3 Training and Testing Added
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
+++ b/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0603EE-90AD-7F47-8876-89EFCEBAAC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{8C0603EE-90AD-7F47-8876-89EFCEBAAC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A0825C1-F5ED-456F-8602-30347E64359E}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="500" windowWidth="26020" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="264" yWindow="96" windowWidth="21732" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -367,7 +367,7 @@
     <t>* P6 blooper</t>
   </si>
   <si>
-    <t>*P6 has 1 dif signer</t>
+    <t>*P6 has 1 diff signer</t>
   </si>
 </sst>
 </file>
@@ -441,6 +441,16 @@
   <dxfs count="7">
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFF0000"/>
       </font>
       <fill>
@@ -451,41 +461,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -506,6 +486,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -793,20 +793,20 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" customWidth="1"/>
-    <col min="10" max="15" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" customWidth="1"/>
+    <col min="10" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -850,7 +850,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -863,7 +863,9 @@
       <c r="D2" s="4">
         <v>24</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4">
+        <v>24</v>
+      </c>
       <c r="F2" s="4">
         <v>25</v>
       </c>
@@ -879,7 +881,9 @@
       <c r="K2" s="4">
         <v>6</v>
       </c>
-      <c r="L2" s="4"/>
+      <c r="L2" s="4">
+        <v>6</v>
+      </c>
       <c r="M2" s="4">
         <v>6</v>
       </c>
@@ -890,7 +894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -903,7 +907,9 @@
       <c r="D3" s="4">
         <v>25</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4">
+        <v>24</v>
+      </c>
       <c r="F3" s="4">
         <v>28</v>
       </c>
@@ -919,7 +925,9 @@
       <c r="K3" s="4">
         <v>6</v>
       </c>
-      <c r="L3" s="4"/>
+      <c r="L3" s="4">
+        <v>6</v>
+      </c>
       <c r="M3" s="4">
         <v>6</v>
       </c>
@@ -930,7 +938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -943,7 +951,9 @@
       <c r="D4" s="4">
         <v>24</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4">
+        <v>24</v>
+      </c>
       <c r="F4" s="4">
         <v>36</v>
       </c>
@@ -959,7 +969,9 @@
       <c r="K4" s="4">
         <v>6</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="L4" s="4">
+        <v>6</v>
+      </c>
       <c r="M4" s="4">
         <v>12</v>
       </c>
@@ -973,7 +985,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -986,7 +998,9 @@
       <c r="D5" s="4">
         <v>24</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4">
+        <v>24</v>
+      </c>
       <c r="F5" s="4">
         <v>25</v>
       </c>
@@ -1002,7 +1016,9 @@
       <c r="K5" s="4">
         <v>6</v>
       </c>
-      <c r="L5" s="4"/>
+      <c r="L5" s="4">
+        <v>6</v>
+      </c>
       <c r="M5" s="4">
         <v>6</v>
       </c>
@@ -1013,7 +1029,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1026,7 +1042,9 @@
       <c r="D6" s="4">
         <v>37</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4">
+        <v>35</v>
+      </c>
       <c r="F6" s="4">
         <v>23</v>
       </c>
@@ -1042,7 +1060,9 @@
       <c r="K6" s="4">
         <v>8</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="L6" s="4">
+        <v>12</v>
+      </c>
       <c r="M6" s="4">
         <v>8</v>
       </c>
@@ -1053,7 +1073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1066,7 +1086,9 @@
       <c r="D7" s="4">
         <v>26</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4">
+        <v>29</v>
+      </c>
       <c r="F7" s="4">
         <v>26</v>
       </c>
@@ -1082,7 +1104,9 @@
       <c r="K7" s="4">
         <v>6</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="L7" s="4">
+        <v>6</v>
+      </c>
       <c r="M7" s="4">
         <v>6</v>
       </c>
@@ -1093,7 +1117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1106,7 +1130,9 @@
       <c r="D8" s="4">
         <v>35</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4">
+        <v>27</v>
+      </c>
       <c r="F8" s="4">
         <v>25</v>
       </c>
@@ -1122,7 +1148,9 @@
       <c r="K8" s="4">
         <v>10</v>
       </c>
-      <c r="L8" s="4"/>
+      <c r="L8" s="4">
+        <v>6</v>
+      </c>
       <c r="M8" s="4">
         <v>6</v>
       </c>
@@ -1133,7 +1161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1146,7 +1174,9 @@
       <c r="D9" s="4">
         <v>24</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4">
+        <v>24</v>
+      </c>
       <c r="F9" s="4">
         <v>28</v>
       </c>
@@ -1162,7 +1192,9 @@
       <c r="K9" s="4">
         <v>6</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="L9" s="4">
+        <v>6</v>
+      </c>
       <c r="M9" s="4">
         <v>6</v>
       </c>
@@ -1173,7 +1205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1186,7 +1218,9 @@
       <c r="D10" s="4">
         <v>24</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4">
+        <v>26</v>
+      </c>
       <c r="F10" s="4">
         <v>24</v>
       </c>
@@ -1202,7 +1236,9 @@
       <c r="K10" s="4">
         <v>6</v>
       </c>
-      <c r="L10" s="4"/>
+      <c r="L10" s="4">
+        <v>6</v>
+      </c>
       <c r="M10" s="4">
         <v>6</v>
       </c>
@@ -1213,7 +1249,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1226,7 +1262,9 @@
       <c r="D11" s="4">
         <v>24</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4">
+        <v>25</v>
+      </c>
       <c r="F11" s="4">
         <v>27</v>
       </c>
@@ -1242,7 +1280,9 @@
       <c r="K11" s="4">
         <v>6</v>
       </c>
-      <c r="L11" s="4"/>
+      <c r="L11" s="4">
+        <v>6</v>
+      </c>
       <c r="M11" s="4">
         <v>6</v>
       </c>
@@ -1253,7 +1293,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1266,7 +1306,9 @@
       <c r="D12" s="4">
         <v>24</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4">
+        <v>26</v>
+      </c>
       <c r="F12" s="4">
         <v>25</v>
       </c>
@@ -1282,7 +1324,9 @@
       <c r="K12" s="4">
         <v>6</v>
       </c>
-      <c r="L12" s="4"/>
+      <c r="L12" s="4">
+        <v>6</v>
+      </c>
       <c r="M12" s="4">
         <v>6</v>
       </c>
@@ -1293,7 +1337,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1306,7 +1350,9 @@
       <c r="D13" s="4">
         <v>26</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4">
+        <v>28</v>
+      </c>
       <c r="F13" s="4">
         <v>25</v>
       </c>
@@ -1322,7 +1368,9 @@
       <c r="K13" s="4">
         <v>6</v>
       </c>
-      <c r="L13" s="4"/>
+      <c r="L13" s="4">
+        <v>6</v>
+      </c>
       <c r="M13" s="4">
         <v>6</v>
       </c>
@@ -1333,7 +1381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1346,7 +1394,9 @@
       <c r="D14" s="4">
         <v>16</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4">
+        <v>28</v>
+      </c>
       <c r="F14" s="4">
         <v>25</v>
       </c>
@@ -1362,7 +1412,9 @@
       <c r="K14" s="4">
         <v>6</v>
       </c>
-      <c r="L14" s="4"/>
+      <c r="L14" s="4">
+        <v>6</v>
+      </c>
       <c r="M14" s="4">
         <v>6</v>
       </c>
@@ -1373,7 +1425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -1386,7 +1438,9 @@
       <c r="D15" s="4">
         <v>25</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4">
+        <v>26</v>
+      </c>
       <c r="F15" s="4">
         <v>24</v>
       </c>
@@ -1402,7 +1456,9 @@
       <c r="K15" s="4">
         <v>6</v>
       </c>
-      <c r="L15" s="4"/>
+      <c r="L15" s="4">
+        <v>6</v>
+      </c>
       <c r="M15" s="4">
         <v>6</v>
       </c>
@@ -1413,7 +1469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1426,7 +1482,9 @@
       <c r="D16" s="4">
         <v>24</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4">
+        <v>25</v>
+      </c>
       <c r="F16" s="4">
         <v>25</v>
       </c>
@@ -1442,7 +1500,9 @@
       <c r="K16" s="4">
         <v>6</v>
       </c>
-      <c r="L16" s="4"/>
+      <c r="L16" s="4">
+        <v>6</v>
+      </c>
       <c r="M16" s="4">
         <v>6</v>
       </c>
@@ -1453,7 +1513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1466,7 +1526,9 @@
       <c r="D17" s="4">
         <v>24</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <v>25</v>
+      </c>
       <c r="F17" s="4">
         <v>25</v>
       </c>
@@ -1482,7 +1544,9 @@
       <c r="K17" s="4">
         <v>6</v>
       </c>
-      <c r="L17" s="4"/>
+      <c r="L17" s="4">
+        <v>6</v>
+      </c>
       <c r="M17" s="4">
         <v>6</v>
       </c>
@@ -1493,7 +1557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1506,7 +1570,9 @@
       <c r="D18" s="4">
         <v>24</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4">
+        <v>30</v>
+      </c>
       <c r="F18" s="4">
         <v>27</v>
       </c>
@@ -1522,7 +1588,9 @@
       <c r="K18" s="4">
         <v>6</v>
       </c>
-      <c r="L18" s="4"/>
+      <c r="L18" s="4">
+        <v>6</v>
+      </c>
       <c r="M18" s="4">
         <v>6</v>
       </c>
@@ -1533,7 +1601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1546,7 +1614,9 @@
       <c r="D19" s="4">
         <v>24</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4">
+        <v>25</v>
+      </c>
       <c r="F19" s="4">
         <v>24</v>
       </c>
@@ -1562,7 +1632,9 @@
       <c r="K19" s="4">
         <v>6</v>
       </c>
-      <c r="L19" s="4"/>
+      <c r="L19" s="4">
+        <v>6</v>
+      </c>
       <c r="M19" s="4">
         <v>6</v>
       </c>
@@ -1573,7 +1645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -1586,7 +1658,9 @@
       <c r="D20" s="4">
         <v>25</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4">
+        <v>26</v>
+      </c>
       <c r="F20" s="4">
         <v>25</v>
       </c>
@@ -1602,7 +1676,9 @@
       <c r="K20" s="4">
         <v>6</v>
       </c>
-      <c r="L20" s="4"/>
+      <c r="L20" s="4">
+        <v>6</v>
+      </c>
       <c r="M20" s="4">
         <v>6</v>
       </c>
@@ -1613,7 +1689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1626,7 +1702,9 @@
       <c r="D21" s="4">
         <v>23</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4">
+        <v>24</v>
+      </c>
       <c r="F21" s="4">
         <v>25</v>
       </c>
@@ -1642,7 +1720,9 @@
       <c r="K21" s="4">
         <v>6</v>
       </c>
-      <c r="L21" s="4"/>
+      <c r="L21" s="4">
+        <v>6</v>
+      </c>
       <c r="M21" s="4">
         <v>6</v>
       </c>
@@ -1653,7 +1733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1666,7 +1746,9 @@
       <c r="D22" s="4">
         <v>24</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4">
+        <v>28</v>
+      </c>
       <c r="F22" s="4">
         <v>24</v>
       </c>
@@ -1682,7 +1764,9 @@
       <c r="K22" s="4">
         <v>6</v>
       </c>
-      <c r="L22" s="4"/>
+      <c r="L22" s="4">
+        <v>6</v>
+      </c>
       <c r="M22" s="4">
         <v>6</v>
       </c>
@@ -1693,7 +1777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1706,7 +1790,9 @@
       <c r="D23" s="4">
         <v>25</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4">
+        <v>24</v>
+      </c>
       <c r="F23" s="4">
         <v>24</v>
       </c>
@@ -1722,7 +1808,9 @@
       <c r="K23" s="4">
         <v>6</v>
       </c>
-      <c r="L23" s="4"/>
+      <c r="L23" s="4">
+        <v>6</v>
+      </c>
       <c r="M23" s="4">
         <v>6</v>
       </c>
@@ -1733,7 +1821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -1746,7 +1834,9 @@
       <c r="D24" s="4">
         <v>25</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4">
+        <v>25</v>
+      </c>
       <c r="F24" s="4">
         <v>24</v>
       </c>
@@ -1762,7 +1852,9 @@
       <c r="K24" s="4">
         <v>6</v>
       </c>
-      <c r="L24" s="4"/>
+      <c r="L24" s="4">
+        <v>6</v>
+      </c>
       <c r="M24" s="4">
         <v>6</v>
       </c>
@@ -1773,7 +1865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -1786,7 +1878,9 @@
       <c r="D25" s="4">
         <v>25</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4">
+        <v>27</v>
+      </c>
       <c r="F25" s="4">
         <v>24</v>
       </c>
@@ -1802,7 +1896,9 @@
       <c r="K25" s="4">
         <v>6</v>
       </c>
-      <c r="L25" s="4"/>
+      <c r="L25" s="4">
+        <v>6</v>
+      </c>
       <c r="M25" s="4">
         <v>6</v>
       </c>
@@ -1813,7 +1909,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -1826,7 +1922,9 @@
       <c r="D26" s="4">
         <v>24</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4">
+        <v>26</v>
+      </c>
       <c r="F26" s="4">
         <v>25</v>
       </c>
@@ -1842,7 +1940,9 @@
       <c r="K26" s="4">
         <v>6</v>
       </c>
-      <c r="L26" s="4"/>
+      <c r="L26" s="4">
+        <v>6</v>
+      </c>
       <c r="M26" s="4">
         <v>6</v>
       </c>
@@ -1853,7 +1953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -1866,7 +1966,9 @@
       <c r="D27" s="4">
         <v>24</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="4">
+        <v>25</v>
+      </c>
       <c r="F27" s="4">
         <v>25</v>
       </c>
@@ -1882,7 +1984,9 @@
       <c r="K27" s="4">
         <v>6</v>
       </c>
-      <c r="L27" s="4"/>
+      <c r="L27" s="4">
+        <v>6</v>
+      </c>
       <c r="M27" s="4">
         <v>6</v>
       </c>
@@ -1893,7 +1997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
@@ -1906,7 +2010,9 @@
       <c r="D28" s="4">
         <v>51</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4">
+        <v>57</v>
+      </c>
       <c r="F28" s="4">
         <v>24</v>
       </c>
@@ -1922,7 +2028,9 @@
       <c r="K28" s="4">
         <v>10</v>
       </c>
-      <c r="L28" s="4"/>
+      <c r="L28" s="4">
+        <v>6</v>
+      </c>
       <c r="M28" s="4">
         <v>6</v>
       </c>
@@ -1933,7 +2041,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -1946,7 +2054,9 @@
       <c r="D29" s="4">
         <v>45</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="4">
+        <v>56</v>
+      </c>
       <c r="F29" s="4">
         <v>24</v>
       </c>
@@ -1962,7 +2072,9 @@
       <c r="K29" s="4">
         <v>16</v>
       </c>
-      <c r="L29" s="4"/>
+      <c r="L29" s="4">
+        <v>6</v>
+      </c>
       <c r="M29" s="4">
         <v>6</v>
       </c>
@@ -1973,7 +2085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -1986,7 +2098,9 @@
       <c r="D30" s="4">
         <v>24</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="4">
+        <v>26</v>
+      </c>
       <c r="F30" s="4">
         <v>24</v>
       </c>
@@ -2002,7 +2116,9 @@
       <c r="K30" s="4">
         <v>6</v>
       </c>
-      <c r="L30" s="4"/>
+      <c r="L30" s="4">
+        <v>6</v>
+      </c>
       <c r="M30" s="4">
         <v>6</v>
       </c>
@@ -2013,7 +2129,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -2026,7 +2142,9 @@
       <c r="D31" s="4">
         <v>25</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4">
+        <v>27</v>
+      </c>
       <c r="F31" s="4">
         <v>24</v>
       </c>
@@ -2045,7 +2163,9 @@
       <c r="K31" s="4">
         <v>6</v>
       </c>
-      <c r="L31" s="4"/>
+      <c r="L31" s="4">
+        <v>6</v>
+      </c>
       <c r="M31" s="4">
         <v>6</v>
       </c>
@@ -2056,7 +2176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -2069,7 +2189,9 @@
       <c r="D32" s="4">
         <v>24</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4">
+        <v>25</v>
+      </c>
       <c r="F32" s="4">
         <v>25</v>
       </c>
@@ -2085,7 +2207,9 @@
       <c r="K32" s="4">
         <v>6</v>
       </c>
-      <c r="L32" s="4"/>
+      <c r="L32" s="4">
+        <v>6</v>
+      </c>
       <c r="M32" s="4">
         <v>6</v>
       </c>
@@ -2096,7 +2220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -2109,7 +2233,9 @@
       <c r="D33" s="4">
         <v>24</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4">
+        <v>24</v>
+      </c>
       <c r="F33" s="4">
         <v>24</v>
       </c>
@@ -2125,7 +2251,9 @@
       <c r="K33" s="4">
         <v>6</v>
       </c>
-      <c r="L33" s="4"/>
+      <c r="L33" s="4">
+        <v>6</v>
+      </c>
       <c r="M33" s="4">
         <v>6</v>
       </c>
@@ -2136,7 +2264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -2149,7 +2277,9 @@
       <c r="D34" s="4">
         <v>24</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4">
+        <v>25</v>
+      </c>
       <c r="F34" s="4">
         <v>24</v>
       </c>
@@ -2165,7 +2295,9 @@
       <c r="K34" s="4">
         <v>6</v>
       </c>
-      <c r="L34" s="4"/>
+      <c r="L34" s="4">
+        <v>6</v>
+      </c>
       <c r="M34" s="4">
         <v>6</v>
       </c>
@@ -2176,7 +2308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -2189,7 +2321,9 @@
       <c r="D35" s="4">
         <v>25</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4">
+        <v>25</v>
+      </c>
       <c r="F35" s="4">
         <v>24</v>
       </c>
@@ -2205,7 +2339,9 @@
       <c r="K35" s="4">
         <v>6</v>
       </c>
-      <c r="L35" s="4"/>
+      <c r="L35" s="4">
+        <v>6</v>
+      </c>
       <c r="M35" s="4">
         <v>6</v>
       </c>
@@ -2216,7 +2352,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
@@ -2229,7 +2365,9 @@
       <c r="D36" s="4">
         <v>24</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4">
+        <v>24</v>
+      </c>
       <c r="F36" s="4">
         <v>25</v>
       </c>
@@ -2245,7 +2383,9 @@
       <c r="K36" s="4">
         <v>6</v>
       </c>
-      <c r="L36" s="4"/>
+      <c r="L36" s="4">
+        <v>6</v>
+      </c>
       <c r="M36" s="4">
         <v>6</v>
       </c>
@@ -2256,7 +2396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -2269,7 +2409,9 @@
       <c r="D37" s="4">
         <v>25</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="4">
+        <v>24</v>
+      </c>
       <c r="F37" s="4">
         <v>24</v>
       </c>
@@ -2285,7 +2427,9 @@
       <c r="K37" s="4">
         <v>6</v>
       </c>
-      <c r="L37" s="4"/>
+      <c r="L37" s="4">
+        <v>6</v>
+      </c>
       <c r="M37" s="4">
         <v>6</v>
       </c>
@@ -2296,7 +2440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -2309,7 +2453,9 @@
       <c r="D38" s="4">
         <v>24</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="4">
+        <v>24</v>
+      </c>
       <c r="F38" s="4">
         <v>24</v>
       </c>
@@ -2325,7 +2471,9 @@
       <c r="K38" s="4">
         <v>6</v>
       </c>
-      <c r="L38" s="4"/>
+      <c r="L38" s="4">
+        <v>6</v>
+      </c>
       <c r="M38" s="4">
         <v>6</v>
       </c>
@@ -2336,7 +2484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -2349,7 +2497,9 @@
       <c r="D39" s="4">
         <v>24</v>
       </c>
-      <c r="E39" s="4"/>
+      <c r="E39" s="4">
+        <v>24</v>
+      </c>
       <c r="F39" s="4">
         <v>24</v>
       </c>
@@ -2365,7 +2515,9 @@
       <c r="K39" s="4">
         <v>6</v>
       </c>
-      <c r="L39" s="4"/>
+      <c r="L39" s="4">
+        <v>6</v>
+      </c>
       <c r="M39" s="4">
         <v>6</v>
       </c>
@@ -2376,7 +2528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
@@ -2389,7 +2541,9 @@
       <c r="D40" s="4">
         <v>24</v>
       </c>
-      <c r="E40" s="4"/>
+      <c r="E40" s="4">
+        <v>24</v>
+      </c>
       <c r="F40" s="4">
         <v>24</v>
       </c>
@@ -2405,7 +2559,9 @@
       <c r="K40" s="4">
         <v>6</v>
       </c>
-      <c r="L40" s="4"/>
+      <c r="L40" s="4">
+        <v>6</v>
+      </c>
       <c r="M40" s="4">
         <v>6</v>
       </c>
@@ -2416,7 +2572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
@@ -2429,7 +2585,9 @@
       <c r="D41" s="4">
         <v>25</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4">
+        <v>24</v>
+      </c>
       <c r="F41" s="4">
         <v>24</v>
       </c>
@@ -2445,7 +2603,9 @@
       <c r="K41" s="4">
         <v>6</v>
       </c>
-      <c r="L41" s="4"/>
+      <c r="L41" s="4">
+        <v>6</v>
+      </c>
       <c r="M41" s="4">
         <v>6</v>
       </c>
@@ -2456,7 +2616,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -2469,7 +2629,9 @@
       <c r="D42" s="4">
         <v>25</v>
       </c>
-      <c r="E42" s="4"/>
+      <c r="E42" s="4">
+        <v>24</v>
+      </c>
       <c r="F42" s="4">
         <v>24</v>
       </c>
@@ -2485,7 +2647,9 @@
       <c r="K42" s="4">
         <v>6</v>
       </c>
-      <c r="L42" s="4"/>
+      <c r="L42" s="4">
+        <v>6</v>
+      </c>
       <c r="M42" s="4">
         <v>6</v>
       </c>
@@ -2496,7 +2660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -2509,7 +2673,9 @@
       <c r="D43" s="4">
         <v>24</v>
       </c>
-      <c r="E43" s="4"/>
+      <c r="E43" s="4">
+        <v>24</v>
+      </c>
       <c r="F43" s="4">
         <v>24</v>
       </c>
@@ -2525,7 +2691,9 @@
       <c r="K43" s="4">
         <v>6</v>
       </c>
-      <c r="L43" s="4"/>
+      <c r="L43" s="4">
+        <v>6</v>
+      </c>
       <c r="M43" s="4">
         <v>6</v>
       </c>
@@ -2536,7 +2704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -2549,7 +2717,9 @@
       <c r="D44" s="4">
         <v>24</v>
       </c>
-      <c r="E44" s="4"/>
+      <c r="E44" s="4">
+        <v>24</v>
+      </c>
       <c r="F44" s="4">
         <v>25</v>
       </c>
@@ -2565,7 +2735,9 @@
       <c r="K44" s="4">
         <v>6</v>
       </c>
-      <c r="L44" s="4"/>
+      <c r="L44" s="4">
+        <v>6</v>
+      </c>
       <c r="M44" s="4">
         <v>6</v>
       </c>
@@ -2576,7 +2748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -2589,7 +2761,9 @@
       <c r="D45" s="4">
         <v>24</v>
       </c>
-      <c r="E45" s="4"/>
+      <c r="E45" s="4">
+        <v>24</v>
+      </c>
       <c r="F45" s="4">
         <v>24</v>
       </c>
@@ -2605,7 +2779,9 @@
       <c r="K45" s="4">
         <v>6</v>
       </c>
-      <c r="L45" s="4"/>
+      <c r="L45" s="4">
+        <v>6</v>
+      </c>
       <c r="M45" s="4">
         <v>6</v>
       </c>
@@ -2616,7 +2792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>90</v>
       </c>
@@ -2629,7 +2805,9 @@
       <c r="D46" s="4">
         <v>24</v>
       </c>
-      <c r="E46" s="4"/>
+      <c r="E46" s="4">
+        <v>24</v>
+      </c>
       <c r="F46" s="4">
         <v>24</v>
       </c>
@@ -2645,7 +2823,9 @@
       <c r="K46" s="4">
         <v>6</v>
       </c>
-      <c r="L46" s="4"/>
+      <c r="L46" s="4">
+        <v>6</v>
+      </c>
       <c r="M46" s="4">
         <v>6</v>
       </c>
@@ -2656,7 +2836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
@@ -2669,7 +2849,9 @@
       <c r="D47" s="4">
         <v>24</v>
       </c>
-      <c r="E47" s="4"/>
+      <c r="E47" s="4">
+        <v>24</v>
+      </c>
       <c r="F47" s="4">
         <v>24</v>
       </c>
@@ -2685,7 +2867,9 @@
       <c r="K47" s="4">
         <v>6</v>
       </c>
-      <c r="L47" s="4"/>
+      <c r="L47" s="4">
+        <v>6</v>
+      </c>
       <c r="M47" s="4">
         <v>6</v>
       </c>
@@ -2696,7 +2880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -2709,7 +2893,9 @@
       <c r="D48" s="4">
         <v>24</v>
       </c>
-      <c r="E48" s="4"/>
+      <c r="E48" s="4">
+        <v>24</v>
+      </c>
       <c r="F48" s="4">
         <v>24</v>
       </c>
@@ -2725,7 +2911,9 @@
       <c r="K48" s="4">
         <v>6</v>
       </c>
-      <c r="L48" s="4"/>
+      <c r="L48" s="4">
+        <v>6</v>
+      </c>
       <c r="M48" s="4">
         <v>6</v>
       </c>
@@ -2736,7 +2924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -2749,7 +2937,9 @@
       <c r="D49" s="4">
         <v>24</v>
       </c>
-      <c r="E49" s="4"/>
+      <c r="E49" s="4">
+        <v>26</v>
+      </c>
       <c r="F49" s="4">
         <v>24</v>
       </c>
@@ -2765,7 +2955,9 @@
       <c r="K49" s="4">
         <v>6</v>
       </c>
-      <c r="L49" s="4"/>
+      <c r="L49" s="4">
+        <v>6</v>
+      </c>
       <c r="M49" s="4">
         <v>6</v>
       </c>
@@ -2776,7 +2968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -2789,7 +2981,9 @@
       <c r="D50" s="4">
         <v>24</v>
       </c>
-      <c r="E50" s="4"/>
+      <c r="E50" s="4">
+        <v>25</v>
+      </c>
       <c r="F50" s="4">
         <v>24</v>
       </c>
@@ -2805,7 +2999,9 @@
       <c r="K50" s="4">
         <v>6</v>
       </c>
-      <c r="L50" s="4"/>
+      <c r="L50" s="4">
+        <v>6</v>
+      </c>
       <c r="M50" s="4">
         <v>6</v>
       </c>
@@ -2816,7 +3012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -2829,7 +3025,9 @@
       <c r="D51" s="4">
         <v>24</v>
       </c>
-      <c r="E51" s="4"/>
+      <c r="E51" s="4">
+        <v>26</v>
+      </c>
       <c r="F51" s="4">
         <v>24</v>
       </c>
@@ -2845,7 +3043,9 @@
       <c r="K51" s="4">
         <v>6</v>
       </c>
-      <c r="L51" s="4"/>
+      <c r="L51" s="4">
+        <v>6</v>
+      </c>
       <c r="M51" s="4">
         <v>6</v>
       </c>
@@ -2858,28 +3058,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:H51">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
-      <formula>21</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="greaterThan">
-      <formula>27</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="between">
       <formula>22</formula>
       <formula>26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>27</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
+      <formula>27</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="lessThan">
+      <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:O51">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
summed the training and testing
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
+++ b/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{8C0603EE-90AD-7F47-8876-89EFCEBAAC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A0825C1-F5ED-456F-8602-30347E64359E}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="264" yWindow="96" windowWidth="21732" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="100" windowWidth="21730" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>SentenceID</t>
   </si>
@@ -368,12 +367,18 @@
   </si>
   <si>
     <t>*P6 has 1 diff signer</t>
+  </si>
+  <si>
+    <t>Sum Training</t>
+  </si>
+  <si>
+    <t>Sum Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -438,7 +443,177 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -789,24 +964,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" customWidth="1"/>
-    <col min="10" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.08984375" customWidth="1"/>
+    <col min="10" max="10" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.08984375" customWidth="1"/>
+    <col min="12" max="17" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -832,25 +1011,31 @@
         <v>107</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S1" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -875,11 +1060,9 @@
       <c r="H2" s="4">
         <v>25</v>
       </c>
-      <c r="J2" s="4">
-        <v>6</v>
-      </c>
-      <c r="K2" s="4">
-        <v>6</v>
+      <c r="J2">
+        <f>SUM(C2:H2)</f>
+        <v>146</v>
       </c>
       <c r="L2" s="4">
         <v>6</v>
@@ -893,8 +1076,18 @@
       <c r="O2" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P2" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>6</v>
+      </c>
+      <c r="S2">
+        <f>SUM(L2:Q2)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -919,11 +1112,9 @@
       <c r="H3" s="4">
         <v>26</v>
       </c>
-      <c r="J3" s="4">
-        <v>6</v>
-      </c>
-      <c r="K3" s="4">
-        <v>6</v>
+      <c r="J3">
+        <f t="shared" ref="J3:J51" si="0">SUM(C3:H3)</f>
+        <v>152</v>
       </c>
       <c r="L3" s="4">
         <v>6</v>
@@ -937,8 +1128,18 @@
       <c r="O3" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P3" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>6</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S51" si="1">SUM(L3:Q3)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -963,29 +1164,37 @@
       <c r="H4" s="4">
         <v>25</v>
       </c>
-      <c r="J4" s="4">
-        <v>6</v>
-      </c>
-      <c r="K4" s="4">
-        <v>6</v>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>157</v>
       </c>
       <c r="L4" s="4">
         <v>6</v>
       </c>
       <c r="M4" s="4">
+        <v>6</v>
+      </c>
+      <c r="N4" s="4">
+        <v>6</v>
+      </c>
+      <c r="O4" s="4">
         <v>12</v>
       </c>
-      <c r="N4" s="4">
-        <v>6</v>
-      </c>
-      <c r="O4" s="4">
-        <v>6</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="P4" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>6</v>
+      </c>
+      <c r="R4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S4">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1010,11 +1219,9 @@
       <c r="H5" s="4">
         <v>24</v>
       </c>
-      <c r="J5" s="4">
-        <v>6</v>
-      </c>
-      <c r="K5" s="4">
-        <v>6</v>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>145</v>
       </c>
       <c r="L5" s="4">
         <v>6</v>
@@ -1028,8 +1235,18 @@
       <c r="O5" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P5" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>6</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1054,26 +1271,34 @@
       <c r="H6" s="4">
         <v>23</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="L6" s="4">
         <v>7</v>
-      </c>
-      <c r="K6" s="4">
-        <v>8</v>
-      </c>
-      <c r="L6" s="4">
-        <v>12</v>
       </c>
       <c r="M6" s="4">
         <v>8</v>
       </c>
       <c r="N6" s="4">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="O6" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="P6" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>6</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1098,15 +1323,13 @@
       <c r="H7" s="4">
         <v>24</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="L7" s="4">
         <v>5</v>
       </c>
-      <c r="K7" s="4">
-        <v>6</v>
-      </c>
-      <c r="L7" s="4">
-        <v>6</v>
-      </c>
       <c r="M7" s="4">
         <v>6</v>
       </c>
@@ -1116,8 +1339,18 @@
       <c r="O7" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P7" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>6</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1142,26 +1375,34 @@
       <c r="H8" s="4">
         <v>24</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="L8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="4">
+      <c r="M8" s="4">
         <v>10</v>
       </c>
-      <c r="L8" s="4">
-        <v>6</v>
-      </c>
-      <c r="M8" s="4">
-        <v>6</v>
-      </c>
       <c r="N8" s="4">
         <v>6</v>
       </c>
       <c r="O8" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P8" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1186,15 +1427,13 @@
       <c r="H9" s="4">
         <v>24</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>157</v>
+      </c>
+      <c r="L9" s="4">
         <v>10</v>
       </c>
-      <c r="K9" s="4">
-        <v>6</v>
-      </c>
-      <c r="L9" s="4">
-        <v>6</v>
-      </c>
       <c r="M9" s="4">
         <v>6</v>
       </c>
@@ -1204,8 +1443,18 @@
       <c r="O9" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P9" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>6</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1230,11 +1479,9 @@
       <c r="H10" s="4">
         <v>24</v>
       </c>
-      <c r="J10" s="4">
-        <v>6</v>
-      </c>
-      <c r="K10" s="4">
-        <v>6</v>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="L10" s="4">
         <v>6</v>
@@ -1248,8 +1495,18 @@
       <c r="O10" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P10" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1274,11 +1531,9 @@
       <c r="H11" s="4">
         <v>24</v>
       </c>
-      <c r="J11" s="4">
-        <v>6</v>
-      </c>
-      <c r="K11" s="4">
-        <v>6</v>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>151</v>
       </c>
       <c r="L11" s="4">
         <v>6</v>
@@ -1292,8 +1547,18 @@
       <c r="O11" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P11" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>6</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1318,11 +1583,9 @@
       <c r="H12" s="4">
         <v>24</v>
       </c>
-      <c r="J12" s="4">
-        <v>6</v>
-      </c>
-      <c r="K12" s="4">
-        <v>6</v>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>147</v>
       </c>
       <c r="L12" s="4">
         <v>6</v>
@@ -1336,8 +1599,18 @@
       <c r="O12" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P12" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>6</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1362,11 +1635,9 @@
       <c r="H13" s="4">
         <v>25</v>
       </c>
-      <c r="J13" s="4">
-        <v>6</v>
-      </c>
-      <c r="K13" s="4">
-        <v>6</v>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>152</v>
       </c>
       <c r="L13" s="4">
         <v>6</v>
@@ -1380,8 +1651,18 @@
       <c r="O13" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P13" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>6</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1406,11 +1687,9 @@
       <c r="H14" s="4">
         <v>24</v>
       </c>
-      <c r="J14" s="4">
-        <v>6</v>
-      </c>
-      <c r="K14" s="4">
-        <v>6</v>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>141</v>
       </c>
       <c r="L14" s="4">
         <v>6</v>
@@ -1424,8 +1703,18 @@
       <c r="O14" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P14" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>6</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -1450,11 +1739,9 @@
       <c r="H15" s="4">
         <v>25</v>
       </c>
-      <c r="J15" s="4">
-        <v>6</v>
-      </c>
-      <c r="K15" s="4">
-        <v>6</v>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>147</v>
       </c>
       <c r="L15" s="4">
         <v>6</v>
@@ -1468,8 +1755,18 @@
       <c r="O15" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P15" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>6</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1494,11 +1791,9 @@
       <c r="H16" s="4">
         <v>24</v>
       </c>
-      <c r="J16" s="4">
-        <v>6</v>
-      </c>
-      <c r="K16" s="4">
-        <v>6</v>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="L16" s="4">
         <v>6</v>
@@ -1512,8 +1807,18 @@
       <c r="O16" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>6</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1538,11 +1843,9 @@
       <c r="H17" s="4">
         <v>24</v>
       </c>
-      <c r="J17" s="4">
-        <v>6</v>
-      </c>
-      <c r="K17" s="4">
-        <v>6</v>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="L17" s="4">
         <v>6</v>
@@ -1556,8 +1859,18 @@
       <c r="O17" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>6</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1582,11 +1895,9 @@
       <c r="H18" s="4">
         <v>24</v>
       </c>
-      <c r="J18" s="4">
-        <v>6</v>
-      </c>
-      <c r="K18" s="4">
-        <v>6</v>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>153</v>
       </c>
       <c r="L18" s="4">
         <v>6</v>
@@ -1600,8 +1911,18 @@
       <c r="O18" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>6</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1626,11 +1947,9 @@
       <c r="H19" s="4">
         <v>24</v>
       </c>
-      <c r="J19" s="4">
-        <v>6</v>
-      </c>
-      <c r="K19" s="4">
-        <v>6</v>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>145</v>
       </c>
       <c r="L19" s="4">
         <v>6</v>
@@ -1644,8 +1963,18 @@
       <c r="O19" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>6</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -1670,11 +1999,9 @@
       <c r="H20" s="4">
         <v>24</v>
       </c>
-      <c r="J20" s="4">
-        <v>6</v>
-      </c>
-      <c r="K20" s="4">
-        <v>6</v>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>148</v>
       </c>
       <c r="L20" s="4">
         <v>6</v>
@@ -1688,8 +2015,18 @@
       <c r="O20" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>6</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1714,11 +2051,9 @@
       <c r="H21" s="4">
         <v>24</v>
       </c>
-      <c r="J21" s="4">
-        <v>6</v>
-      </c>
-      <c r="K21" s="4">
-        <v>6</v>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>143</v>
       </c>
       <c r="L21" s="4">
         <v>6</v>
@@ -1732,8 +2067,18 @@
       <c r="O21" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>6</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1758,11 +2103,9 @@
       <c r="H22" s="4">
         <v>24</v>
       </c>
-      <c r="J22" s="4">
-        <v>6</v>
-      </c>
-      <c r="K22" s="4">
-        <v>6</v>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>148</v>
       </c>
       <c r="L22" s="4">
         <v>6</v>
@@ -1776,8 +2119,18 @@
       <c r="O22" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>6</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1802,11 +2155,9 @@
       <c r="H23" s="4">
         <v>25</v>
       </c>
-      <c r="J23" s="4">
-        <v>6</v>
-      </c>
-      <c r="K23" s="4">
-        <v>6</v>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="L23" s="4">
         <v>6</v>
@@ -1820,8 +2171,18 @@
       <c r="O23" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>6</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -1846,11 +2207,9 @@
       <c r="H24" s="4">
         <v>26</v>
       </c>
-      <c r="J24" s="4">
-        <v>6</v>
-      </c>
-      <c r="K24" s="4">
-        <v>6</v>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>148</v>
       </c>
       <c r="L24" s="4">
         <v>6</v>
@@ -1864,8 +2223,18 @@
       <c r="O24" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>6</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -1890,11 +2259,9 @@
       <c r="H25" s="4">
         <v>24</v>
       </c>
-      <c r="J25" s="4">
-        <v>6</v>
-      </c>
-      <c r="K25" s="4">
-        <v>6</v>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>148</v>
       </c>
       <c r="L25" s="4">
         <v>6</v>
@@ -1908,8 +2275,18 @@
       <c r="O25" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>6</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -1934,11 +2311,9 @@
       <c r="H26" s="4">
         <v>26</v>
       </c>
-      <c r="J26" s="4">
-        <v>6</v>
-      </c>
-      <c r="K26" s="4">
-        <v>6</v>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>149</v>
       </c>
       <c r="L26" s="4">
         <v>6</v>
@@ -1952,8 +2327,18 @@
       <c r="O26" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>6</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -1978,11 +2363,9 @@
       <c r="H27" s="4">
         <v>25</v>
       </c>
-      <c r="J27" s="4">
-        <v>6</v>
-      </c>
-      <c r="K27" s="4">
-        <v>6</v>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>147</v>
       </c>
       <c r="L27" s="4">
         <v>6</v>
@@ -1996,8 +2379,18 @@
       <c r="O27" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>6</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
@@ -2022,26 +2415,34 @@
       <c r="H28" s="4">
         <v>24</v>
       </c>
-      <c r="J28" s="4">
-        <v>6</v>
-      </c>
-      <c r="K28" s="4">
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>204</v>
+      </c>
+      <c r="L28" s="4">
+        <v>6</v>
+      </c>
+      <c r="M28" s="4">
         <v>10</v>
       </c>
-      <c r="L28" s="4">
-        <v>6</v>
-      </c>
-      <c r="M28" s="4">
-        <v>6</v>
-      </c>
       <c r="N28" s="4">
         <v>6</v>
       </c>
       <c r="O28" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>6</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -2066,26 +2467,34 @@
       <c r="H29" s="4">
         <v>24</v>
       </c>
-      <c r="J29" s="4">
-        <v>6</v>
-      </c>
-      <c r="K29" s="4">
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>197</v>
+      </c>
+      <c r="L29" s="4">
+        <v>6</v>
+      </c>
+      <c r="M29" s="4">
         <v>16</v>
       </c>
-      <c r="L29" s="4">
-        <v>6</v>
-      </c>
-      <c r="M29" s="4">
-        <v>6</v>
-      </c>
       <c r="N29" s="4">
         <v>6</v>
       </c>
       <c r="O29" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>6</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -2110,11 +2519,9 @@
       <c r="H30" s="4">
         <v>24</v>
       </c>
-      <c r="J30" s="4">
-        <v>6</v>
-      </c>
-      <c r="K30" s="4">
-        <v>6</v>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="L30" s="4">
         <v>6</v>
@@ -2128,8 +2535,18 @@
       <c r="O30" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>6</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -2157,11 +2574,9 @@
       <c r="I31" t="s">
         <v>114</v>
       </c>
-      <c r="J31" s="4">
-        <v>6</v>
-      </c>
-      <c r="K31" s="4">
-        <v>6</v>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>148</v>
       </c>
       <c r="L31" s="4">
         <v>6</v>
@@ -2175,8 +2590,18 @@
       <c r="O31" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P31" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>6</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -2201,11 +2626,9 @@
       <c r="H32" s="4">
         <v>24</v>
       </c>
-      <c r="J32" s="4">
-        <v>6</v>
-      </c>
-      <c r="K32" s="4">
-        <v>6</v>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="L32" s="4">
         <v>6</v>
@@ -2219,8 +2642,18 @@
       <c r="O32" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P32" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>6</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -2245,11 +2678,9 @@
       <c r="H33" s="4">
         <v>24</v>
       </c>
-      <c r="J33" s="4">
-        <v>6</v>
-      </c>
-      <c r="K33" s="4">
-        <v>6</v>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>144</v>
       </c>
       <c r="L33" s="4">
         <v>6</v>
@@ -2263,8 +2694,18 @@
       <c r="O33" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P33" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>6</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -2289,11 +2730,9 @@
       <c r="H34" s="4">
         <v>25</v>
       </c>
-      <c r="J34" s="4">
-        <v>6</v>
-      </c>
-      <c r="K34" s="4">
-        <v>6</v>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="L34" s="4">
         <v>6</v>
@@ -2307,8 +2746,18 @@
       <c r="O34" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P34" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>6</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -2333,11 +2782,9 @@
       <c r="H35" s="4">
         <v>24</v>
       </c>
-      <c r="J35" s="4">
-        <v>6</v>
-      </c>
-      <c r="K35" s="4">
-        <v>6</v>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>145</v>
       </c>
       <c r="L35" s="4">
         <v>6</v>
@@ -2351,8 +2798,18 @@
       <c r="O35" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P35" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>6</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
@@ -2377,11 +2834,9 @@
       <c r="H36" s="4">
         <v>24</v>
       </c>
-      <c r="J36" s="4">
-        <v>6</v>
-      </c>
-      <c r="K36" s="4">
-        <v>6</v>
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>145</v>
       </c>
       <c r="L36" s="4">
         <v>6</v>
@@ -2395,8 +2850,18 @@
       <c r="O36" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P36" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>6</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -2421,11 +2886,9 @@
       <c r="H37" s="4">
         <v>24</v>
       </c>
-      <c r="J37" s="4">
-        <v>6</v>
-      </c>
-      <c r="K37" s="4">
-        <v>6</v>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="L37" s="4">
         <v>6</v>
@@ -2439,8 +2902,18 @@
       <c r="O37" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P37" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>6</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -2465,11 +2938,9 @@
       <c r="H38" s="4">
         <v>24</v>
       </c>
-      <c r="J38" s="4">
-        <v>6</v>
-      </c>
-      <c r="K38" s="4">
-        <v>6</v>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>144</v>
       </c>
       <c r="L38" s="4">
         <v>6</v>
@@ -2483,8 +2954,18 @@
       <c r="O38" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P38" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>6</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -2509,11 +2990,9 @@
       <c r="H39" s="4">
         <v>24</v>
       </c>
-      <c r="J39" s="4">
-        <v>6</v>
-      </c>
-      <c r="K39" s="4">
-        <v>6</v>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>144</v>
       </c>
       <c r="L39" s="4">
         <v>6</v>
@@ -2527,8 +3006,18 @@
       <c r="O39" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P39" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>6</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
@@ -2553,11 +3042,9 @@
       <c r="H40" s="4">
         <v>24</v>
       </c>
-      <c r="J40" s="4">
-        <v>6</v>
-      </c>
-      <c r="K40" s="4">
-        <v>6</v>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>144</v>
       </c>
       <c r="L40" s="4">
         <v>6</v>
@@ -2571,8 +3058,18 @@
       <c r="O40" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P40" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q40" s="4">
+        <v>6</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
@@ -2597,11 +3094,9 @@
       <c r="H41" s="4">
         <v>24</v>
       </c>
-      <c r="J41" s="4">
-        <v>6</v>
-      </c>
-      <c r="K41" s="4">
-        <v>6</v>
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>145</v>
       </c>
       <c r="L41" s="4">
         <v>6</v>
@@ -2615,8 +3110,18 @@
       <c r="O41" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P41" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q41" s="4">
+        <v>6</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -2641,11 +3146,9 @@
       <c r="H42" s="4">
         <v>24</v>
       </c>
-      <c r="J42" s="4">
-        <v>6</v>
-      </c>
-      <c r="K42" s="4">
-        <v>6</v>
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>145</v>
       </c>
       <c r="L42" s="4">
         <v>6</v>
@@ -2659,8 +3162,18 @@
       <c r="O42" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P42" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q42" s="4">
+        <v>6</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -2685,11 +3198,9 @@
       <c r="H43" s="4">
         <v>24</v>
       </c>
-      <c r="J43" s="4">
-        <v>6</v>
-      </c>
-      <c r="K43" s="4">
-        <v>6</v>
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>143</v>
       </c>
       <c r="L43" s="4">
         <v>6</v>
@@ -2703,8 +3214,18 @@
       <c r="O43" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P43" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q43" s="4">
+        <v>6</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -2729,11 +3250,9 @@
       <c r="H44" s="4">
         <v>24</v>
       </c>
-      <c r="J44" s="4">
-        <v>6</v>
-      </c>
-      <c r="K44" s="4">
-        <v>6</v>
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>145</v>
       </c>
       <c r="L44" s="4">
         <v>6</v>
@@ -2747,8 +3266,18 @@
       <c r="O44" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P44" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q44" s="4">
+        <v>6</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -2773,15 +3302,13 @@
       <c r="H45" s="4">
         <v>24</v>
       </c>
-      <c r="J45" s="4">
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="L45" s="4">
         <v>5</v>
       </c>
-      <c r="K45" s="4">
-        <v>6</v>
-      </c>
-      <c r="L45" s="4">
-        <v>6</v>
-      </c>
       <c r="M45" s="4">
         <v>6</v>
       </c>
@@ -2791,8 +3318,18 @@
       <c r="O45" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P45" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q45" s="4">
+        <v>6</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>90</v>
       </c>
@@ -2817,11 +3354,9 @@
       <c r="H46" s="4">
         <v>24</v>
       </c>
-      <c r="J46" s="4">
-        <v>6</v>
-      </c>
-      <c r="K46" s="4">
-        <v>6</v>
+      <c r="J46">
+        <f t="shared" si="0"/>
+        <v>144</v>
       </c>
       <c r="L46" s="4">
         <v>6</v>
@@ -2835,8 +3370,18 @@
       <c r="O46" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P46" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q46" s="4">
+        <v>6</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
@@ -2861,11 +3406,9 @@
       <c r="H47" s="4">
         <v>24</v>
       </c>
-      <c r="J47" s="4">
-        <v>6</v>
-      </c>
-      <c r="K47" s="4">
-        <v>6</v>
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>144</v>
       </c>
       <c r="L47" s="4">
         <v>6</v>
@@ -2879,8 +3422,18 @@
       <c r="O47" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P47" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q47" s="4">
+        <v>6</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -2905,11 +3458,9 @@
       <c r="H48" s="4">
         <v>24</v>
       </c>
-      <c r="J48" s="4">
-        <v>6</v>
-      </c>
-      <c r="K48" s="4">
-        <v>6</v>
+      <c r="J48">
+        <f t="shared" si="0"/>
+        <v>144</v>
       </c>
       <c r="L48" s="4">
         <v>6</v>
@@ -2923,8 +3474,18 @@
       <c r="O48" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P48" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>6</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -2949,11 +3510,9 @@
       <c r="H49" s="4">
         <v>24</v>
       </c>
-      <c r="J49" s="4">
-        <v>6</v>
-      </c>
-      <c r="K49" s="4">
-        <v>6</v>
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="L49" s="4">
         <v>6</v>
@@ -2967,8 +3526,18 @@
       <c r="O49" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P49" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q49" s="4">
+        <v>6</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -2993,11 +3562,9 @@
       <c r="H50" s="4">
         <v>24</v>
       </c>
-      <c r="J50" s="4">
-        <v>6</v>
-      </c>
-      <c r="K50" s="4">
-        <v>6</v>
+      <c r="J50">
+        <f t="shared" si="0"/>
+        <v>145</v>
       </c>
       <c r="L50" s="4">
         <v>6</v>
@@ -3011,8 +3578,18 @@
       <c r="O50" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P50" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>6</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -3037,11 +3614,9 @@
       <c r="H51" s="4">
         <v>24</v>
       </c>
-      <c r="J51" s="4">
-        <v>6</v>
-      </c>
-      <c r="K51" s="4">
-        <v>6</v>
+      <c r="J51">
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="L51" s="4">
         <v>6</v>
@@ -3054,33 +3629,53 @@
       </c>
       <c r="O51" s="4">
         <v>6</v>
+      </c>
+      <c r="P51" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>6</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="1"/>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:H51">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="between">
       <formula>22</formula>
       <formula>26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="greaterThan">
       <formula>27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="lessThan">
       <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:O51">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+  <conditionalFormatting sqref="L2:Q51">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="notEqual">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J51">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="lessThan">
+      <formula>144</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:S51">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>36</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added total number of videos to excel sheet
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
+++ b/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_6A3D5EE78DEAF43025225605F153ABF103B6BC61" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB60BE4A-CFE1-40E2-AF91-366C15B63BE3}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="100" windowWidth="21730" windowHeight="13620"/>
+    <workbookView xWindow="264" yWindow="96" windowWidth="21732" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="120">
   <si>
     <t>SentenceID</t>
   </si>
@@ -373,12 +385,18 @@
   </si>
   <si>
     <t>Sum Testing</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>All Videos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -443,17 +461,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -491,146 +499,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -964,28 +832,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.08984375" customWidth="1"/>
-    <col min="10" max="10" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.08984375" customWidth="1"/>
-    <col min="12" max="17" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" customWidth="1"/>
+    <col min="12" max="17" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +903,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1087,7 +955,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1139,7 +1007,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1194,7 +1062,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1246,7 +1114,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1298,7 +1166,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1350,7 +1218,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1402,7 +1270,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1454,7 +1322,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1506,7 +1374,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1558,7 +1426,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1610,7 +1478,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1662,7 +1530,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1714,7 +1582,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -1766,7 +1634,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1818,7 +1686,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1870,7 +1738,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1922,7 +1790,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1974,7 +1842,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -2026,7 +1894,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -2078,7 +1946,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -2130,7 +1998,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -2182,7 +2050,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -2234,7 +2102,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -2286,7 +2154,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -2338,7 +2206,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -2390,7 +2258,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
@@ -2442,7 +2310,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -2494,7 +2362,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -2546,7 +2414,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -2601,7 +2469,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -2653,7 +2521,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -2705,7 +2573,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -2757,7 +2625,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -2809,7 +2677,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
@@ -2861,7 +2729,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -2913,7 +2781,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -2965,7 +2833,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -3017,7 +2885,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
@@ -3069,7 +2937,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
@@ -3121,7 +2989,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -3173,7 +3041,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -3225,7 +3093,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -3277,7 +3145,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -3329,7 +3197,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>90</v>
       </c>
@@ -3381,7 +3249,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
@@ -3433,7 +3301,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -3485,7 +3353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -3537,7 +3405,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -3589,7 +3457,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -3641,39 +3509,64 @@
         <v>36</v>
       </c>
     </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I52" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J52" s="4">
+        <f>SUM(J2:J51)</f>
+        <v>7480</v>
+      </c>
+      <c r="R52" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="S52" s="4">
+        <f>SUM(S2:S51)</f>
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I56" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J56" s="4">
+        <f>SUM(J52:S52)</f>
+        <v>9321</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C2:H51">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="between">
       <formula>22</formula>
       <formula>26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="greaterThan">
       <formula>27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="12" operator="lessThan">
       <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J52">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+      <formula>144</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L2:Q51">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J51">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="lessThan">
-      <formula>144</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S51">
+  <conditionalFormatting sqref="S2:S52">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>36</formula>
     </cfRule>

</xml_diff>

<commit_message>
added a new sheet to show new vids counts
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
+++ b/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_6A3D5EE78DEAF43025225605F153ABF103B6BC61" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB60BE4A-CFE1-40E2-AF91-366C15B63BE3}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="264" yWindow="96" windowWidth="21732" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="100" windowWidth="21730" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="After keeping max 26 vids" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="120">
   <si>
     <t>SentenceID</t>
   </si>
@@ -396,7 +396,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -461,7 +461,97 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -832,28 +922,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView topLeftCell="B1" zoomScale="52" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" customWidth="1"/>
-    <col min="12" max="17" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.08984375" customWidth="1"/>
+    <col min="10" max="10" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.08984375" customWidth="1"/>
+    <col min="12" max="17" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -903,7 +993,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -955,7 +1045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1007,7 +1097,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1062,7 +1152,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1204,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1166,7 +1256,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1218,7 +1308,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1270,7 +1360,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1322,7 +1412,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1374,7 +1464,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1426,7 +1516,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1478,7 +1568,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1530,7 +1620,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1582,7 +1672,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -1634,7 +1724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1686,7 +1776,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1738,7 +1828,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1790,7 +1880,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1842,7 +1932,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -1894,7 +1984,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1946,7 +2036,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1998,7 +2088,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -2050,7 +2140,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -2102,7 +2192,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -2154,7 +2244,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -2206,7 +2296,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -2258,7 +2348,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
@@ -2310,7 +2400,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -2362,7 +2452,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -2414,7 +2504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -2469,7 +2559,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -2521,7 +2611,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -2573,7 +2663,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -2625,7 +2715,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -2677,7 +2767,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
@@ -2729,7 +2819,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -2781,7 +2871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -2833,7 +2923,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -2885,7 +2975,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
@@ -2937,7 +3027,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
@@ -2989,7 +3079,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -3041,7 +3131,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -3093,7 +3183,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -3145,7 +3235,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -3197,7 +3287,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>90</v>
       </c>
@@ -3249,7 +3339,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
@@ -3301,7 +3391,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -3353,7 +3443,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -3405,7 +3495,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -3457,7 +3547,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -3509,7 +3599,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I52" s="4" t="s">
         <v>118</v>
       </c>
@@ -3525,7 +3615,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I56" s="4" t="s">
         <v>119</v>
       </c>
@@ -3536,20 +3626,2759 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:H51">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="between">
       <formula>22</formula>
       <formula>26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
       <formula>27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="greaterThan">
       <formula>27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="lessThan">
+      <formula>21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J52">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThan">
+      <formula>144</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:Q51">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="notEqual">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:S52">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
+      <formula>36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.08984375" customWidth="1"/>
+    <col min="10" max="10" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.08984375" customWidth="1"/>
+    <col min="12" max="17" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4">
+        <v>24</v>
+      </c>
+      <c r="E2" s="4">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4">
+        <v>24</v>
+      </c>
+      <c r="H2" s="4">
+        <v>25</v>
+      </c>
+      <c r="J2">
+        <f>SUM(C2:H2)</f>
+        <v>146</v>
+      </c>
+      <c r="L2" s="4">
+        <v>6</v>
+      </c>
+      <c r="M2" s="4">
+        <v>6</v>
+      </c>
+      <c r="N2" s="4">
+        <v>6</v>
+      </c>
+      <c r="O2" s="4">
+        <v>6</v>
+      </c>
+      <c r="P2" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>6</v>
+      </c>
+      <c r="S2">
+        <f>SUM(L2:Q2)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4">
+        <v>25</v>
+      </c>
+      <c r="E3" s="4">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4">
+        <v>24</v>
+      </c>
+      <c r="H3" s="4">
+        <v>26</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J51" si="0">SUM(C3:H3)</f>
+        <v>150</v>
+      </c>
+      <c r="L3" s="4">
+        <v>6</v>
+      </c>
+      <c r="M3" s="4">
+        <v>6</v>
+      </c>
+      <c r="N3" s="4">
+        <v>6</v>
+      </c>
+      <c r="O3" s="4">
+        <v>6</v>
+      </c>
+      <c r="P3" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>6</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S51" si="1">SUM(L3:Q3)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>24</v>
+      </c>
+      <c r="D4" s="4">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4">
+        <v>24</v>
+      </c>
+      <c r="F4" s="4">
+        <v>26</v>
+      </c>
+      <c r="G4" s="4">
+        <v>24</v>
+      </c>
+      <c r="H4" s="4">
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="L4" s="4">
+        <v>6</v>
+      </c>
+      <c r="M4" s="4">
+        <v>6</v>
+      </c>
+      <c r="N4" s="4">
+        <v>6</v>
+      </c>
+      <c r="O4" s="4">
+        <v>13</v>
+      </c>
+      <c r="P4" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4">
+        <v>25</v>
+      </c>
+      <c r="G5" s="4">
+        <v>24</v>
+      </c>
+      <c r="H5" s="4">
+        <v>24</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="L5" s="4">
+        <v>6</v>
+      </c>
+      <c r="M5" s="4">
+        <v>6</v>
+      </c>
+      <c r="N5" s="4">
+        <v>6</v>
+      </c>
+      <c r="O5" s="4">
+        <v>6</v>
+      </c>
+      <c r="P5" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>6</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4">
+        <v>26</v>
+      </c>
+      <c r="E6" s="4">
+        <v>26</v>
+      </c>
+      <c r="F6" s="4">
+        <v>23</v>
+      </c>
+      <c r="G6" s="4">
+        <v>24</v>
+      </c>
+      <c r="H6" s="4">
+        <v>23</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="L6" s="4">
+        <v>7</v>
+      </c>
+      <c r="M6" s="4">
+        <v>8</v>
+      </c>
+      <c r="N6" s="4">
+        <v>12</v>
+      </c>
+      <c r="O6" s="4">
+        <v>8</v>
+      </c>
+      <c r="P6" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>6</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4">
+        <v>24</v>
+      </c>
+      <c r="H7" s="4">
+        <v>24</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="L7" s="4">
+        <v>5</v>
+      </c>
+      <c r="M7" s="4">
+        <v>6</v>
+      </c>
+      <c r="N7" s="4">
+        <v>6</v>
+      </c>
+      <c r="O7" s="4">
+        <v>6</v>
+      </c>
+      <c r="P7" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>6</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4">
+        <v>26</v>
+      </c>
+      <c r="E8" s="4">
+        <v>26</v>
+      </c>
+      <c r="F8" s="4">
+        <v>25</v>
+      </c>
+      <c r="G8" s="4">
+        <v>24</v>
+      </c>
+      <c r="H8" s="4">
+        <v>24</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>151</v>
+      </c>
+      <c r="L8" s="4">
+        <v>10</v>
+      </c>
+      <c r="M8" s="4">
+        <v>10</v>
+      </c>
+      <c r="N8" s="4">
+        <v>6</v>
+      </c>
+      <c r="O8" s="4">
+        <v>6</v>
+      </c>
+      <c r="P8" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4">
+        <v>24</v>
+      </c>
+      <c r="E9" s="4">
+        <v>24</v>
+      </c>
+      <c r="F9" s="4">
+        <v>26</v>
+      </c>
+      <c r="G9" s="4">
+        <v>24</v>
+      </c>
+      <c r="H9" s="4">
+        <v>24</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="L9" s="4">
+        <v>10</v>
+      </c>
+      <c r="M9" s="4">
+        <v>6</v>
+      </c>
+      <c r="N9" s="4">
+        <v>6</v>
+      </c>
+      <c r="O9" s="4">
+        <v>6</v>
+      </c>
+      <c r="P9" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>6</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4">
+        <v>24</v>
+      </c>
+      <c r="E10" s="4">
+        <v>26</v>
+      </c>
+      <c r="F10" s="4">
+        <v>24</v>
+      </c>
+      <c r="G10" s="4">
+        <v>24</v>
+      </c>
+      <c r="H10" s="4">
+        <v>24</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L10" s="4">
+        <v>6</v>
+      </c>
+      <c r="M10" s="4">
+        <v>6</v>
+      </c>
+      <c r="N10" s="4">
+        <v>6</v>
+      </c>
+      <c r="O10" s="4">
+        <v>6</v>
+      </c>
+      <c r="P10" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="4">
+        <v>26</v>
+      </c>
+      <c r="D11" s="4">
+        <v>24</v>
+      </c>
+      <c r="E11" s="4">
+        <v>25</v>
+      </c>
+      <c r="F11" s="4">
+        <v>26</v>
+      </c>
+      <c r="G11" s="4">
+        <v>24</v>
+      </c>
+      <c r="H11" s="4">
+        <v>24</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="L11" s="4">
+        <v>6</v>
+      </c>
+      <c r="M11" s="4">
+        <v>6</v>
+      </c>
+      <c r="N11" s="4">
+        <v>6</v>
+      </c>
+      <c r="O11" s="4">
+        <v>6</v>
+      </c>
+      <c r="P11" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>6</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4">
+        <v>24</v>
+      </c>
+      <c r="D12" s="4">
+        <v>24</v>
+      </c>
+      <c r="E12" s="4">
+        <v>26</v>
+      </c>
+      <c r="F12" s="4">
+        <v>25</v>
+      </c>
+      <c r="G12" s="4">
+        <v>24</v>
+      </c>
+      <c r="H12" s="4">
+        <v>24</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="L12" s="4">
+        <v>6</v>
+      </c>
+      <c r="M12" s="4">
+        <v>6</v>
+      </c>
+      <c r="N12" s="4">
+        <v>6</v>
+      </c>
+      <c r="O12" s="4">
+        <v>6</v>
+      </c>
+      <c r="P12" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>6</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4">
+        <v>24</v>
+      </c>
+      <c r="D13" s="4">
+        <v>26</v>
+      </c>
+      <c r="E13" s="4">
+        <v>26</v>
+      </c>
+      <c r="F13" s="4">
+        <v>25</v>
+      </c>
+      <c r="G13" s="4">
+        <v>24</v>
+      </c>
+      <c r="H13" s="4">
+        <v>25</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="L13" s="4">
+        <v>6</v>
+      </c>
+      <c r="M13" s="4">
+        <v>6</v>
+      </c>
+      <c r="N13" s="4">
+        <v>6</v>
+      </c>
+      <c r="O13" s="4">
+        <v>6</v>
+      </c>
+      <c r="P13" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>6</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4">
+        <v>24</v>
+      </c>
+      <c r="D14" s="4">
+        <v>16</v>
+      </c>
+      <c r="E14" s="4">
+        <v>26</v>
+      </c>
+      <c r="F14" s="4">
+        <v>25</v>
+      </c>
+      <c r="G14" s="4">
+        <v>24</v>
+      </c>
+      <c r="H14" s="4">
+        <v>24</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="L14" s="4">
+        <v>6</v>
+      </c>
+      <c r="M14" s="4">
+        <v>6</v>
+      </c>
+      <c r="N14" s="4">
+        <v>6</v>
+      </c>
+      <c r="O14" s="4">
+        <v>6</v>
+      </c>
+      <c r="P14" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>6</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="4">
+        <v>23</v>
+      </c>
+      <c r="D15" s="4">
+        <v>25</v>
+      </c>
+      <c r="E15" s="4">
+        <v>26</v>
+      </c>
+      <c r="F15" s="4">
+        <v>24</v>
+      </c>
+      <c r="G15" s="4">
+        <v>24</v>
+      </c>
+      <c r="H15" s="4">
+        <v>25</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="L15" s="4">
+        <v>6</v>
+      </c>
+      <c r="M15" s="4">
+        <v>6</v>
+      </c>
+      <c r="N15" s="4">
+        <v>6</v>
+      </c>
+      <c r="O15" s="4">
+        <v>6</v>
+      </c>
+      <c r="P15" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>6</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="4">
+        <v>24</v>
+      </c>
+      <c r="D16" s="4">
+        <v>24</v>
+      </c>
+      <c r="E16" s="4">
+        <v>25</v>
+      </c>
+      <c r="F16" s="4">
+        <v>25</v>
+      </c>
+      <c r="G16" s="4">
+        <v>24</v>
+      </c>
+      <c r="H16" s="4">
+        <v>24</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L16" s="4">
+        <v>6</v>
+      </c>
+      <c r="M16" s="4">
+        <v>6</v>
+      </c>
+      <c r="N16" s="4">
+        <v>6</v>
+      </c>
+      <c r="O16" s="4">
+        <v>6</v>
+      </c>
+      <c r="P16" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>6</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="4">
+        <v>24</v>
+      </c>
+      <c r="D17" s="4">
+        <v>24</v>
+      </c>
+      <c r="E17" s="4">
+        <v>25</v>
+      </c>
+      <c r="F17" s="4">
+        <v>25</v>
+      </c>
+      <c r="G17" s="4">
+        <v>24</v>
+      </c>
+      <c r="H17" s="4">
+        <v>24</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L17" s="4">
+        <v>6</v>
+      </c>
+      <c r="M17" s="4">
+        <v>6</v>
+      </c>
+      <c r="N17" s="4">
+        <v>6</v>
+      </c>
+      <c r="O17" s="4">
+        <v>6</v>
+      </c>
+      <c r="P17" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>6</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="4">
+        <v>24</v>
+      </c>
+      <c r="D18" s="4">
+        <v>24</v>
+      </c>
+      <c r="E18" s="4">
+        <v>26</v>
+      </c>
+      <c r="F18" s="4">
+        <v>26</v>
+      </c>
+      <c r="G18" s="4">
+        <v>24</v>
+      </c>
+      <c r="H18" s="4">
+        <v>24</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="L18" s="4">
+        <v>6</v>
+      </c>
+      <c r="M18" s="4">
+        <v>6</v>
+      </c>
+      <c r="N18" s="4">
+        <v>6</v>
+      </c>
+      <c r="O18" s="4">
+        <v>6</v>
+      </c>
+      <c r="P18" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>6</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="4">
+        <v>24</v>
+      </c>
+      <c r="D19" s="4">
+        <v>24</v>
+      </c>
+      <c r="E19" s="4">
+        <v>25</v>
+      </c>
+      <c r="F19" s="4">
+        <v>24</v>
+      </c>
+      <c r="G19" s="4">
+        <v>24</v>
+      </c>
+      <c r="H19" s="4">
+        <v>24</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="L19" s="4">
+        <v>6</v>
+      </c>
+      <c r="M19" s="4">
+        <v>6</v>
+      </c>
+      <c r="N19" s="4">
+        <v>6</v>
+      </c>
+      <c r="O19" s="4">
+        <v>6</v>
+      </c>
+      <c r="P19" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>6</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="4">
+        <v>24</v>
+      </c>
+      <c r="D20" s="4">
+        <v>25</v>
+      </c>
+      <c r="E20" s="4">
+        <v>26</v>
+      </c>
+      <c r="F20" s="4">
+        <v>25</v>
+      </c>
+      <c r="G20" s="4">
+        <v>24</v>
+      </c>
+      <c r="H20" s="4">
+        <v>24</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="L20" s="4">
+        <v>6</v>
+      </c>
+      <c r="M20" s="4">
+        <v>6</v>
+      </c>
+      <c r="N20" s="4">
+        <v>6</v>
+      </c>
+      <c r="O20" s="4">
+        <v>6</v>
+      </c>
+      <c r="P20" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>6</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="4">
+        <v>23</v>
+      </c>
+      <c r="D21" s="4">
+        <v>23</v>
+      </c>
+      <c r="E21" s="4">
+        <v>24</v>
+      </c>
+      <c r="F21" s="4">
+        <v>25</v>
+      </c>
+      <c r="G21" s="4">
+        <v>24</v>
+      </c>
+      <c r="H21" s="4">
+        <v>24</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="L21" s="4">
+        <v>6</v>
+      </c>
+      <c r="M21" s="4">
+        <v>6</v>
+      </c>
+      <c r="N21" s="4">
+        <v>6</v>
+      </c>
+      <c r="O21" s="4">
+        <v>6</v>
+      </c>
+      <c r="P21" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>6</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="4">
+        <v>24</v>
+      </c>
+      <c r="D22" s="4">
+        <v>24</v>
+      </c>
+      <c r="E22" s="4">
+        <v>26</v>
+      </c>
+      <c r="F22" s="4">
+        <v>24</v>
+      </c>
+      <c r="G22" s="4">
+        <v>24</v>
+      </c>
+      <c r="H22" s="4">
+        <v>24</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L22" s="4">
+        <v>6</v>
+      </c>
+      <c r="M22" s="4">
+        <v>6</v>
+      </c>
+      <c r="N22" s="4">
+        <v>6</v>
+      </c>
+      <c r="O22" s="4">
+        <v>6</v>
+      </c>
+      <c r="P22" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>6</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="4">
+        <v>24</v>
+      </c>
+      <c r="D23" s="4">
+        <v>25</v>
+      </c>
+      <c r="E23" s="4">
+        <v>24</v>
+      </c>
+      <c r="F23" s="4">
+        <v>24</v>
+      </c>
+      <c r="G23" s="4">
+        <v>24</v>
+      </c>
+      <c r="H23" s="4">
+        <v>25</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L23" s="4">
+        <v>6</v>
+      </c>
+      <c r="M23" s="4">
+        <v>6</v>
+      </c>
+      <c r="N23" s="4">
+        <v>6</v>
+      </c>
+      <c r="O23" s="4">
+        <v>6</v>
+      </c>
+      <c r="P23" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>6</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="4">
+        <v>24</v>
+      </c>
+      <c r="D24" s="4">
+        <v>25</v>
+      </c>
+      <c r="E24" s="4">
+        <v>25</v>
+      </c>
+      <c r="F24" s="4">
+        <v>24</v>
+      </c>
+      <c r="G24" s="4">
+        <v>24</v>
+      </c>
+      <c r="H24" s="4">
+        <v>26</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="L24" s="4">
+        <v>6</v>
+      </c>
+      <c r="M24" s="4">
+        <v>6</v>
+      </c>
+      <c r="N24" s="4">
+        <v>6</v>
+      </c>
+      <c r="O24" s="4">
+        <v>6</v>
+      </c>
+      <c r="P24" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>6</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="4">
+        <v>24</v>
+      </c>
+      <c r="D25" s="4">
+        <v>25</v>
+      </c>
+      <c r="E25" s="4">
+        <v>26</v>
+      </c>
+      <c r="F25" s="4">
+        <v>24</v>
+      </c>
+      <c r="G25" s="4">
+        <v>24</v>
+      </c>
+      <c r="H25" s="4">
+        <v>24</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="L25" s="4">
+        <v>6</v>
+      </c>
+      <c r="M25" s="4">
+        <v>6</v>
+      </c>
+      <c r="N25" s="4">
+        <v>6</v>
+      </c>
+      <c r="O25" s="4">
+        <v>6</v>
+      </c>
+      <c r="P25" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>6</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="4">
+        <v>24</v>
+      </c>
+      <c r="D26" s="4">
+        <v>24</v>
+      </c>
+      <c r="E26" s="4">
+        <v>26</v>
+      </c>
+      <c r="F26" s="4">
+        <v>25</v>
+      </c>
+      <c r="G26" s="4">
+        <v>24</v>
+      </c>
+      <c r="H26" s="4">
+        <v>26</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="L26" s="4">
+        <v>6</v>
+      </c>
+      <c r="M26" s="4">
+        <v>6</v>
+      </c>
+      <c r="N26" s="4">
+        <v>6</v>
+      </c>
+      <c r="O26" s="4">
+        <v>6</v>
+      </c>
+      <c r="P26" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>6</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="4">
+        <v>24</v>
+      </c>
+      <c r="D27" s="4">
+        <v>24</v>
+      </c>
+      <c r="E27" s="4">
+        <v>25</v>
+      </c>
+      <c r="F27" s="4">
+        <v>25</v>
+      </c>
+      <c r="G27" s="4">
+        <v>24</v>
+      </c>
+      <c r="H27" s="4">
+        <v>25</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="L27" s="4">
+        <v>6</v>
+      </c>
+      <c r="M27" s="4">
+        <v>6</v>
+      </c>
+      <c r="N27" s="4">
+        <v>6</v>
+      </c>
+      <c r="O27" s="4">
+        <v>6</v>
+      </c>
+      <c r="P27" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>6</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="4">
+        <v>24</v>
+      </c>
+      <c r="D28" s="4">
+        <v>26</v>
+      </c>
+      <c r="E28" s="4">
+        <v>26</v>
+      </c>
+      <c r="F28" s="4">
+        <v>24</v>
+      </c>
+      <c r="G28" s="4">
+        <v>24</v>
+      </c>
+      <c r="H28" s="4">
+        <v>24</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="L28" s="4">
+        <v>6</v>
+      </c>
+      <c r="M28" s="4">
+        <v>10</v>
+      </c>
+      <c r="N28" s="4">
+        <v>6</v>
+      </c>
+      <c r="O28" s="4">
+        <v>6</v>
+      </c>
+      <c r="P28" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>6</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="4">
+        <v>24</v>
+      </c>
+      <c r="D29" s="4">
+        <v>26</v>
+      </c>
+      <c r="E29" s="4">
+        <v>26</v>
+      </c>
+      <c r="F29" s="4">
+        <v>24</v>
+      </c>
+      <c r="G29" s="4">
+        <v>24</v>
+      </c>
+      <c r="H29" s="4">
+        <v>24</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="L29" s="4">
+        <v>6</v>
+      </c>
+      <c r="M29" s="4">
+        <v>16</v>
+      </c>
+      <c r="N29" s="4">
+        <v>6</v>
+      </c>
+      <c r="O29" s="4">
+        <v>6</v>
+      </c>
+      <c r="P29" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>6</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="4">
+        <v>24</v>
+      </c>
+      <c r="D30" s="4">
+        <v>24</v>
+      </c>
+      <c r="E30" s="4">
+        <v>26</v>
+      </c>
+      <c r="F30" s="4">
+        <v>24</v>
+      </c>
+      <c r="G30" s="4">
+        <v>24</v>
+      </c>
+      <c r="H30" s="4">
+        <v>24</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L30" s="4">
+        <v>6</v>
+      </c>
+      <c r="M30" s="4">
+        <v>6</v>
+      </c>
+      <c r="N30" s="4">
+        <v>6</v>
+      </c>
+      <c r="O30" s="4">
+        <v>6</v>
+      </c>
+      <c r="P30" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>6</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="4">
+        <v>24</v>
+      </c>
+      <c r="D31" s="4">
+        <v>25</v>
+      </c>
+      <c r="E31" s="4">
+        <v>26</v>
+      </c>
+      <c r="F31" s="4">
+        <v>24</v>
+      </c>
+      <c r="G31" s="4">
+        <v>24</v>
+      </c>
+      <c r="H31" s="4">
+        <v>23</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L31" s="4">
+        <v>6</v>
+      </c>
+      <c r="M31" s="4">
+        <v>6</v>
+      </c>
+      <c r="N31" s="4">
+        <v>6</v>
+      </c>
+      <c r="O31" s="4">
+        <v>6</v>
+      </c>
+      <c r="P31" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>6</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="4">
+        <v>24</v>
+      </c>
+      <c r="D32" s="4">
+        <v>24</v>
+      </c>
+      <c r="E32" s="4">
+        <v>25</v>
+      </c>
+      <c r="F32" s="4">
+        <v>25</v>
+      </c>
+      <c r="G32" s="4">
+        <v>24</v>
+      </c>
+      <c r="H32" s="4">
+        <v>24</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L32" s="4">
+        <v>6</v>
+      </c>
+      <c r="M32" s="4">
+        <v>6</v>
+      </c>
+      <c r="N32" s="4">
+        <v>6</v>
+      </c>
+      <c r="O32" s="4">
+        <v>6</v>
+      </c>
+      <c r="P32" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>6</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="4">
+        <v>24</v>
+      </c>
+      <c r="D33" s="4">
+        <v>24</v>
+      </c>
+      <c r="E33" s="4">
+        <v>24</v>
+      </c>
+      <c r="F33" s="4">
+        <v>24</v>
+      </c>
+      <c r="G33" s="4">
+        <v>24</v>
+      </c>
+      <c r="H33" s="4">
+        <v>24</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="L33" s="4">
+        <v>6</v>
+      </c>
+      <c r="M33" s="4">
+        <v>6</v>
+      </c>
+      <c r="N33" s="4">
+        <v>6</v>
+      </c>
+      <c r="O33" s="4">
+        <v>6</v>
+      </c>
+      <c r="P33" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>6</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="4">
+        <v>24</v>
+      </c>
+      <c r="D34" s="4">
+        <v>24</v>
+      </c>
+      <c r="E34" s="4">
+        <v>25</v>
+      </c>
+      <c r="F34" s="4">
+        <v>24</v>
+      </c>
+      <c r="G34" s="4">
+        <v>24</v>
+      </c>
+      <c r="H34" s="4">
+        <v>25</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L34" s="4">
+        <v>6</v>
+      </c>
+      <c r="M34" s="4">
+        <v>6</v>
+      </c>
+      <c r="N34" s="4">
+        <v>6</v>
+      </c>
+      <c r="O34" s="4">
+        <v>6</v>
+      </c>
+      <c r="P34" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>6</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="4">
+        <v>23</v>
+      </c>
+      <c r="D35" s="4">
+        <v>25</v>
+      </c>
+      <c r="E35" s="4">
+        <v>25</v>
+      </c>
+      <c r="F35" s="4">
+        <v>24</v>
+      </c>
+      <c r="G35" s="4">
+        <v>24</v>
+      </c>
+      <c r="H35" s="4">
+        <v>24</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="L35" s="4">
+        <v>6</v>
+      </c>
+      <c r="M35" s="4">
+        <v>6</v>
+      </c>
+      <c r="N35" s="4">
+        <v>6</v>
+      </c>
+      <c r="O35" s="4">
+        <v>6</v>
+      </c>
+      <c r="P35" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>6</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="4">
+        <v>24</v>
+      </c>
+      <c r="D36" s="4">
+        <v>24</v>
+      </c>
+      <c r="E36" s="4">
+        <v>24</v>
+      </c>
+      <c r="F36" s="4">
+        <v>25</v>
+      </c>
+      <c r="G36" s="4">
+        <v>24</v>
+      </c>
+      <c r="H36" s="4">
+        <v>24</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="L36" s="4">
+        <v>6</v>
+      </c>
+      <c r="M36" s="4">
+        <v>6</v>
+      </c>
+      <c r="N36" s="4">
+        <v>6</v>
+      </c>
+      <c r="O36" s="4">
+        <v>6</v>
+      </c>
+      <c r="P36" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>6</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="4">
+        <v>25</v>
+      </c>
+      <c r="D37" s="4">
+        <v>25</v>
+      </c>
+      <c r="E37" s="4">
+        <v>24</v>
+      </c>
+      <c r="F37" s="4">
+        <v>24</v>
+      </c>
+      <c r="G37" s="4">
+        <v>24</v>
+      </c>
+      <c r="H37" s="4">
+        <v>24</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L37" s="4">
+        <v>6</v>
+      </c>
+      <c r="M37" s="4">
+        <v>6</v>
+      </c>
+      <c r="N37" s="4">
+        <v>6</v>
+      </c>
+      <c r="O37" s="4">
+        <v>6</v>
+      </c>
+      <c r="P37" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>6</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="4">
+        <v>24</v>
+      </c>
+      <c r="D38" s="4">
+        <v>24</v>
+      </c>
+      <c r="E38" s="4">
+        <v>24</v>
+      </c>
+      <c r="F38" s="4">
+        <v>24</v>
+      </c>
+      <c r="G38" s="4">
+        <v>24</v>
+      </c>
+      <c r="H38" s="4">
+        <v>24</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="L38" s="4">
+        <v>6</v>
+      </c>
+      <c r="M38" s="4">
+        <v>6</v>
+      </c>
+      <c r="N38" s="4">
+        <v>6</v>
+      </c>
+      <c r="O38" s="4">
+        <v>6</v>
+      </c>
+      <c r="P38" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>6</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="4">
+        <v>24</v>
+      </c>
+      <c r="D39" s="4">
+        <v>24</v>
+      </c>
+      <c r="E39" s="4">
+        <v>24</v>
+      </c>
+      <c r="F39" s="4">
+        <v>24</v>
+      </c>
+      <c r="G39" s="4">
+        <v>24</v>
+      </c>
+      <c r="H39" s="4">
+        <v>24</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="L39" s="4">
+        <v>6</v>
+      </c>
+      <c r="M39" s="4">
+        <v>6</v>
+      </c>
+      <c r="N39" s="4">
+        <v>6</v>
+      </c>
+      <c r="O39" s="4">
+        <v>6</v>
+      </c>
+      <c r="P39" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>6</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="4">
+        <v>24</v>
+      </c>
+      <c r="D40" s="4">
+        <v>24</v>
+      </c>
+      <c r="E40" s="4">
+        <v>24</v>
+      </c>
+      <c r="F40" s="4">
+        <v>24</v>
+      </c>
+      <c r="G40" s="4">
+        <v>24</v>
+      </c>
+      <c r="H40" s="4">
+        <v>24</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="L40" s="4">
+        <v>6</v>
+      </c>
+      <c r="M40" s="4">
+        <v>6</v>
+      </c>
+      <c r="N40" s="4">
+        <v>6</v>
+      </c>
+      <c r="O40" s="4">
+        <v>6</v>
+      </c>
+      <c r="P40" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q40" s="4">
+        <v>6</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="4">
+        <v>24</v>
+      </c>
+      <c r="D41" s="4">
+        <v>25</v>
+      </c>
+      <c r="E41" s="4">
+        <v>24</v>
+      </c>
+      <c r="F41" s="4">
+        <v>24</v>
+      </c>
+      <c r="G41" s="4">
+        <v>24</v>
+      </c>
+      <c r="H41" s="4">
+        <v>24</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="L41" s="4">
+        <v>6</v>
+      </c>
+      <c r="M41" s="4">
+        <v>6</v>
+      </c>
+      <c r="N41" s="4">
+        <v>6</v>
+      </c>
+      <c r="O41" s="4">
+        <v>6</v>
+      </c>
+      <c r="P41" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q41" s="4">
+        <v>6</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="4">
+        <v>24</v>
+      </c>
+      <c r="D42" s="4">
+        <v>25</v>
+      </c>
+      <c r="E42" s="4">
+        <v>24</v>
+      </c>
+      <c r="F42" s="4">
+        <v>24</v>
+      </c>
+      <c r="G42" s="4">
+        <v>24</v>
+      </c>
+      <c r="H42" s="4">
+        <v>24</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="L42" s="4">
+        <v>6</v>
+      </c>
+      <c r="M42" s="4">
+        <v>6</v>
+      </c>
+      <c r="N42" s="4">
+        <v>6</v>
+      </c>
+      <c r="O42" s="4">
+        <v>6</v>
+      </c>
+      <c r="P42" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q42" s="4">
+        <v>6</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="4">
+        <v>24</v>
+      </c>
+      <c r="D43" s="4">
+        <v>24</v>
+      </c>
+      <c r="E43" s="4">
+        <v>24</v>
+      </c>
+      <c r="F43" s="4">
+        <v>24</v>
+      </c>
+      <c r="G43" s="4">
+        <v>23</v>
+      </c>
+      <c r="H43" s="4">
+        <v>24</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="L43" s="4">
+        <v>6</v>
+      </c>
+      <c r="M43" s="4">
+        <v>6</v>
+      </c>
+      <c r="N43" s="4">
+        <v>6</v>
+      </c>
+      <c r="O43" s="4">
+        <v>6</v>
+      </c>
+      <c r="P43" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q43" s="4">
+        <v>6</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="4">
+        <v>24</v>
+      </c>
+      <c r="D44" s="4">
+        <v>24</v>
+      </c>
+      <c r="E44" s="4">
+        <v>24</v>
+      </c>
+      <c r="F44" s="4">
+        <v>25</v>
+      </c>
+      <c r="G44" s="4">
+        <v>24</v>
+      </c>
+      <c r="H44" s="4">
+        <v>24</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="L44" s="4">
+        <v>6</v>
+      </c>
+      <c r="M44" s="4">
+        <v>6</v>
+      </c>
+      <c r="N44" s="4">
+        <v>6</v>
+      </c>
+      <c r="O44" s="4">
+        <v>6</v>
+      </c>
+      <c r="P44" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q44" s="4">
+        <v>6</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="4">
+        <v>24</v>
+      </c>
+      <c r="D45" s="4">
+        <v>24</v>
+      </c>
+      <c r="E45" s="4">
+        <v>24</v>
+      </c>
+      <c r="F45" s="4">
+        <v>24</v>
+      </c>
+      <c r="G45" s="4">
+        <v>24</v>
+      </c>
+      <c r="H45" s="4">
+        <v>24</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="L45" s="4">
+        <v>5</v>
+      </c>
+      <c r="M45" s="4">
+        <v>6</v>
+      </c>
+      <c r="N45" s="4">
+        <v>6</v>
+      </c>
+      <c r="O45" s="4">
+        <v>6</v>
+      </c>
+      <c r="P45" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q45" s="4">
+        <v>6</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="4">
+        <v>24</v>
+      </c>
+      <c r="D46" s="4">
+        <v>24</v>
+      </c>
+      <c r="E46" s="4">
+        <v>24</v>
+      </c>
+      <c r="F46" s="4">
+        <v>24</v>
+      </c>
+      <c r="G46" s="4">
+        <v>24</v>
+      </c>
+      <c r="H46" s="4">
+        <v>24</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="L46" s="4">
+        <v>6</v>
+      </c>
+      <c r="M46" s="4">
+        <v>6</v>
+      </c>
+      <c r="N46" s="4">
+        <v>6</v>
+      </c>
+      <c r="O46" s="4">
+        <v>6</v>
+      </c>
+      <c r="P46" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q46" s="4">
+        <v>6</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="4">
+        <v>24</v>
+      </c>
+      <c r="D47" s="4">
+        <v>24</v>
+      </c>
+      <c r="E47" s="4">
+        <v>24</v>
+      </c>
+      <c r="F47" s="4">
+        <v>24</v>
+      </c>
+      <c r="G47" s="4">
+        <v>24</v>
+      </c>
+      <c r="H47" s="4">
+        <v>24</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="L47" s="4">
+        <v>6</v>
+      </c>
+      <c r="M47" s="4">
+        <v>6</v>
+      </c>
+      <c r="N47" s="4">
+        <v>6</v>
+      </c>
+      <c r="O47" s="4">
+        <v>6</v>
+      </c>
+      <c r="P47" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q47" s="4">
+        <v>6</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="4">
+        <v>24</v>
+      </c>
+      <c r="D48" s="4">
+        <v>24</v>
+      </c>
+      <c r="E48" s="4">
+        <v>24</v>
+      </c>
+      <c r="F48" s="4">
+        <v>24</v>
+      </c>
+      <c r="G48" s="4">
+        <v>24</v>
+      </c>
+      <c r="H48" s="4">
+        <v>24</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="L48" s="4">
+        <v>6</v>
+      </c>
+      <c r="M48" s="4">
+        <v>6</v>
+      </c>
+      <c r="N48" s="4">
+        <v>6</v>
+      </c>
+      <c r="O48" s="4">
+        <v>6</v>
+      </c>
+      <c r="P48" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>6</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="4">
+        <v>24</v>
+      </c>
+      <c r="D49" s="4">
+        <v>24</v>
+      </c>
+      <c r="E49" s="4">
+        <v>26</v>
+      </c>
+      <c r="F49" s="4">
+        <v>24</v>
+      </c>
+      <c r="G49" s="4">
+        <v>24</v>
+      </c>
+      <c r="H49" s="4">
+        <v>24</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L49" s="4">
+        <v>6</v>
+      </c>
+      <c r="M49" s="4">
+        <v>6</v>
+      </c>
+      <c r="N49" s="4">
+        <v>6</v>
+      </c>
+      <c r="O49" s="4">
+        <v>6</v>
+      </c>
+      <c r="P49" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q49" s="4">
+        <v>6</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="4">
+        <v>24</v>
+      </c>
+      <c r="D50" s="4">
+        <v>24</v>
+      </c>
+      <c r="E50" s="4">
+        <v>25</v>
+      </c>
+      <c r="F50" s="4">
+        <v>24</v>
+      </c>
+      <c r="G50" s="4">
+        <v>24</v>
+      </c>
+      <c r="H50" s="4">
+        <v>24</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="L50" s="4">
+        <v>6</v>
+      </c>
+      <c r="M50" s="4">
+        <v>6</v>
+      </c>
+      <c r="N50" s="4">
+        <v>6</v>
+      </c>
+      <c r="O50" s="4">
+        <v>6</v>
+      </c>
+      <c r="P50" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>6</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="4">
+        <v>24</v>
+      </c>
+      <c r="D51" s="4">
+        <v>24</v>
+      </c>
+      <c r="E51" s="4">
+        <v>26</v>
+      </c>
+      <c r="F51" s="4">
+        <v>24</v>
+      </c>
+      <c r="G51" s="4">
+        <v>24</v>
+      </c>
+      <c r="H51" s="4">
+        <v>24</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="L51" s="4">
+        <v>6</v>
+      </c>
+      <c r="M51" s="4">
+        <v>6</v>
+      </c>
+      <c r="N51" s="4">
+        <v>6</v>
+      </c>
+      <c r="O51" s="4">
+        <v>6</v>
+      </c>
+      <c r="P51" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>6</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="I52" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J52" s="4">
+        <f>SUM(J2:J51)</f>
+        <v>7301</v>
+      </c>
+      <c r="R52" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="S52" s="4">
+        <f>SUM(S2:S51)</f>
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="I56" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J56" s="4">
+        <f>SUM(J52:S52)</f>
+        <v>9142</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:H51">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="between">
+      <formula>22</formula>
+      <formula>26</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>27</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="greaterThan">
+      <formula>27</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="lessThan">
       <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3572,6 +6401,5 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
included total stack frames we're using for training
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
+++ b/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="122">
   <si>
     <t>SentenceID</t>
   </si>
@@ -391,6 +391,12 @@
   </si>
   <si>
     <t>All Videos</t>
+  </si>
+  <si>
+    <t>Num Words</t>
+  </si>
+  <si>
+    <t>Training Size</t>
   </si>
 </sst>
 </file>
@@ -449,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -457,6 +463,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3668,10 +3677,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S56"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="G29" zoomScale="86" workbookViewId="0">
+      <selection activeCell="S53" sqref="S53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3686,9 +3695,10 @@
     <col min="12" max="17" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3737,8 +3747,14 @@
       <c r="S1" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3789,8 +3805,15 @@
         <f>SUM(L2:Q2)</f>
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U2" s="5">
+        <v>2</v>
+      </c>
+      <c r="W2">
+        <f>U2*(C2+D2+E2+F2+G2+H2)</f>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -3841,8 +3864,15 @@
         <f t="shared" ref="S3:S51" si="1">SUM(L3:Q3)</f>
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U3" s="5">
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W51" si="2">U3*(C3+D3+E3+F3+G3+H3)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -3893,8 +3923,15 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U4" s="5">
+        <v>4</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="2"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -3945,8 +3982,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U5" s="5">
+        <v>5</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="2"/>
+        <v>725</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3997,8 +4041,15 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U6" s="5">
+        <v>5</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="2"/>
+        <v>725</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -4049,8 +4100,15 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U7" s="5">
+        <v>5</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="2"/>
+        <v>745</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -4101,8 +4159,15 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U8" s="5">
+        <v>5</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="2"/>
+        <v>755</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -4153,8 +4218,15 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U9" s="5">
+        <v>3</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="2"/>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -4205,8 +4277,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U10" s="5">
+        <v>3</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="2"/>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -4257,8 +4336,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U11" s="5">
+        <v>2</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="2"/>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -4309,8 +4395,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U12" s="5">
+        <v>4</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="2"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -4361,8 +4454,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U13" s="5">
+        <v>3</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="2"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -4413,8 +4513,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U14" s="5">
+        <v>2</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="2"/>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -4465,8 +4572,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U15" s="5">
+        <v>2</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="2"/>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -4517,8 +4631,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U16" s="5">
+        <v>3</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="2"/>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -4569,8 +4690,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U17" s="5">
+        <v>3</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="2"/>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -4621,8 +4749,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U18" s="5">
+        <v>2</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="2"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -4673,8 +4808,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U19" s="5">
+        <v>4</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="2"/>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -4725,8 +4867,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U20" s="5">
+        <v>3</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="2"/>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -4777,8 +4926,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U21" s="5">
+        <v>3</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="2"/>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -4829,8 +4985,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U22" s="5">
+        <v>4</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="2"/>
+        <v>584</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -4881,8 +5044,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U23" s="5">
+        <v>2</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -4933,8 +5103,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U24" s="5">
+        <v>3</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="2"/>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -4985,8 +5162,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U25" s="5">
+        <v>5</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="2"/>
+        <v>735</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -5037,8 +5221,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U26" s="5">
+        <v>5</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="2"/>
+        <v>745</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -5089,8 +5280,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U27" s="5">
+        <v>5</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="2"/>
+        <v>735</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
@@ -5141,8 +5339,15 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U28" s="5">
+        <v>2</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="2"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -5193,8 +5398,15 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U29" s="5">
+        <v>2</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="2"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -5245,8 +5457,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U30" s="5">
+        <v>4</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="2"/>
+        <v>584</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -5297,8 +5516,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U31" s="5">
+        <v>4</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="2"/>
+        <v>584</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -5349,8 +5575,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U32" s="5">
+        <v>5</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="2"/>
+        <v>730</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -5401,8 +5634,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U33" s="5">
+        <v>4</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="2"/>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -5453,8 +5693,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U34" s="5">
+        <v>3</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="2"/>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -5505,8 +5752,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U35" s="5">
+        <v>2</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="2"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
@@ -5557,8 +5811,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U36" s="5">
+        <v>3</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="2"/>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -5609,8 +5870,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U37" s="5">
+        <v>3</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="2"/>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -5661,8 +5929,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U38" s="5">
+        <v>3</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="2"/>
+        <v>432</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -5713,8 +5988,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U39" s="5">
+        <v>3</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="2"/>
+        <v>432</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
@@ -5765,8 +6047,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U40" s="5">
+        <v>2</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
@@ -5817,8 +6106,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U41" s="5">
+        <v>2</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="2"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -5869,8 +6165,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U42" s="5">
+        <v>2</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="2"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -5921,8 +6224,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U43" s="5">
+        <v>3</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="2"/>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -5973,8 +6283,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U44" s="5">
+        <v>2</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="2"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -6025,8 +6342,15 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U45" s="5">
+        <v>2</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>90</v>
       </c>
@@ -6077,8 +6401,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U46" s="5">
+        <v>2</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
@@ -6129,8 +6460,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U47" s="5">
+        <v>2</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="2"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -6181,8 +6519,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U48" s="5">
+        <v>4</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="2"/>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -6233,8 +6578,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U49" s="5">
+        <v>2</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -6285,8 +6637,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U50" s="5">
+        <v>2</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="2"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -6337,8 +6696,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U51" s="5">
+        <v>3</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="2"/>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
       <c r="I52" s="4" t="s">
         <v>118</v>
       </c>
@@ -6353,8 +6719,15 @@
         <f>SUM(S2:S51)</f>
         <v>1841</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V52" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="W52" s="4">
+        <f>SUM(W2:W51)</f>
+        <v>22658</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
       <c r="I56" s="4" t="s">
         <v>119</v>
       </c>
@@ -6401,5 +6774,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up all python notebooks
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
+++ b/Dataset Excel Sheets/Num of Vids Train and Test.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="127">
   <si>
     <t>SentenceID</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>Cumulative</t>
+  </si>
+  <si>
+    <t>* there's -1</t>
   </si>
 </sst>
 </file>
@@ -3728,8 +3731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F33" zoomScale="86" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54:Q54"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="86" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6763,11 +6766,11 @@
         <v>1203</v>
       </c>
       <c r="D52" s="4">
-        <f t="shared" ref="D52:H52" si="3">SUM(D2:D51)</f>
+        <f>SUM(D2:D51)</f>
         <v>1214</v>
       </c>
       <c r="E52" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D52:H52" si="3">SUM(E2:E51)</f>
         <v>1248</v>
       </c>
       <c r="F52" s="4">
@@ -6882,6 +6885,9 @@
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="D54" t="s">
+        <v>126</v>
+      </c>
       <c r="S54" s="8"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.35">

</xml_diff>